<commit_message>
Random Forest implemented, csv generated
</commit_message>
<xml_diff>
--- a/BANDEJA DO PERIODO.xlsx
+++ b/BANDEJA DO PERIODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/980841a2e24dade8/Profissional/The Coffee/Operação/2.Gestão da Qualidade/Bandejas/Bandejas semanais/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Repositories\bonus_bandejas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3540" documentId="13_ncr:4000b_{D3240E66-DB17-44F6-81B1-0D6B85E22F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E76A7A94-5D17-4A4E-9C55-AA1B68E8EE35}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E7D2D2-F013-4289-9A3A-762465F99C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="período" sheetId="4" r:id="rId1"/>
@@ -22,8 +22,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId7"/>
-    <pivotCache cacheId="34" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="82">
   <si>
     <t xml:space="preserve">               New / App / Cold</t>
   </si>
@@ -1812,9 +1812,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gabriel Bezerra de Melo Silva" refreshedDate="45240.872888194448" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="286" xr:uid="{9B5733B9-D351-4D08-9F8A-CB6331F2432F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gabriel Bezerra de Melo Silva" refreshedDate="45280.880935416666" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="321" xr:uid="{9B5733B9-D351-4D08-9F8A-CB6331F2432F}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J287" sheet="baristas"/>
+    <worksheetSource ref="A1:J322" sheet="baristas"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Ano" numFmtId="0">
@@ -2782,7 +2782,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="286">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="321">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -6215,12 +6215,432 @@
     <n v="0"/>
     <n v="9"/>
   </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="12"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="12"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="16"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="12"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="11"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="19"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="9"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="16"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{993A75B1-F664-4E54-94B9-642F255C2CD9}" name="Tabela dinâmica5" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{993A75B1-F664-4E54-94B9-642F255C2CD9}" name="Tabela dinâmica5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G53" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" showAll="0">
       <items count="3">
@@ -6298,7 +6718,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="43">
+  <rowItems count="50">
     <i>
       <x/>
     </i>
@@ -6425,6 +6845,27 @@
     <i>
       <x v="42"/>
     </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -6476,7 +6917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2D0BEC72-E2E3-4364-A338-C437D8B6491F}" name="Tabela dinâmica1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2D0BEC72-E2E3-4364-A338-C437D8B6491F}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -6664,8 +7105,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}" name="Tabela1" displayName="Tabela1" ref="A1:AI72" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" dataCellStyle="Porcentagem">
-  <autoFilter ref="A1:AI72" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}" name="Tabela1" displayName="Tabela1" ref="A1:AI77" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" dataCellStyle="Porcentagem">
+  <autoFilter ref="A1:AI77" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}"/>
   <tableColumns count="35">
     <tableColumn id="35" xr3:uid="{D883C38E-9A1B-4018-9C05-1951B621A1A9}" name="Ano" dataDxfId="39"/>
     <tableColumn id="1" xr3:uid="{58D0E2F2-6E36-4066-8A1E-F3A3770AE0D4}" name="Semana" dataDxfId="38"/>
@@ -6744,8 +7185,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}" name="Tabela2" displayName="Tabela2" ref="A1:J72" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:J72" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}" name="Tabela2" displayName="Tabela2" ref="A1:J79" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:J79" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{B3A7EC93-D052-476E-A7D0-7F9FEE82E6EB}" name="Ano" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{8907E03F-0276-4E6E-BA76-03A5F7E7ABA8}" name="Semana" dataDxfId="3"/>
@@ -6767,8 +7208,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}" name="Tabela3" displayName="Tabela3" ref="A1:J287" totalsRowShown="0">
-  <autoFilter ref="A1:J287" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}" name="Tabela3" displayName="Tabela3" ref="A1:J322" totalsRowShown="0">
+  <autoFilter ref="A1:J322" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{19C2ECCC-C5CA-4CBA-9A19-FCC8487A8CC6}" name="Ano"/>
     <tableColumn id="1" xr3:uid="{42E434D7-D8A5-4430-8FC7-28848FD6B96A}" name="Semana"/>
@@ -7095,13 +7536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AK72"/>
+  <dimension ref="A1:AK77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S67" sqref="S67:S72"/>
+      <selection pane="bottomRight" activeCell="K73" sqref="K73:Q77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16190,6 +16631,621 @@
         <v>1.0198477767006608</v>
       </c>
     </row>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A73" s="49">
+        <v>2023</v>
+      </c>
+      <c r="B73" s="49">
+        <v>45</v>
+      </c>
+      <c r="C73" s="13">
+        <v>43</v>
+      </c>
+      <c r="D73" s="13">
+        <v>486</v>
+      </c>
+      <c r="E73" s="13">
+        <v>78</v>
+      </c>
+      <c r="F73" s="13">
+        <v>125</v>
+      </c>
+      <c r="G73" s="13">
+        <v>9</v>
+      </c>
+      <c r="H73" s="13">
+        <v>191</v>
+      </c>
+      <c r="I73" s="13">
+        <v>2</v>
+      </c>
+      <c r="J73" s="50">
+        <f t="shared" ref="J73:J77" si="149">SUM(C73:I73)</f>
+        <v>934</v>
+      </c>
+      <c r="K73" s="3">
+        <v>507.7465195479482</v>
+      </c>
+      <c r="L73" s="3">
+        <v>6165.2674300271892</v>
+      </c>
+      <c r="M73" s="3">
+        <v>1587.0930174970829</v>
+      </c>
+      <c r="N73" s="3">
+        <v>819.44626599165531</v>
+      </c>
+      <c r="O73" s="3">
+        <v>139.87000049393401</v>
+      </c>
+      <c r="P73" s="3">
+        <v>454.20434174666781</v>
+      </c>
+      <c r="Q73" s="3">
+        <v>192</v>
+      </c>
+      <c r="R73" s="38">
+        <f t="shared" ref="R73:R77" si="150">SUM(K73:Q73)</f>
+        <v>9865.6275753044793</v>
+      </c>
+      <c r="S73" s="39">
+        <f>(C73*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C73:H73)</f>
+        <v>11.114407898658484</v>
+      </c>
+      <c r="T73" s="58">
+        <f t="shared" ref="T73:T77" si="151">$K73/SUM($K73:$Q73)</f>
+        <v>5.1466215977879926E-2</v>
+      </c>
+      <c r="U73" s="58">
+        <f t="shared" ref="U73:U77" si="152">L73/SUM($K73:$Q73)</f>
+        <v>0.62492399829282153</v>
+      </c>
+      <c r="V73" s="58">
+        <f t="shared" ref="V73:Y77" si="153">M73/SUM($K$2:$Q$2)</f>
+        <v>0.4518144160767848</v>
+      </c>
+      <c r="W73" s="58">
+        <f t="shared" si="153"/>
+        <v>0.23328036359154475</v>
+      </c>
+      <c r="X73" s="58">
+        <f t="shared" si="153"/>
+        <v>3.9818260116529398E-2</v>
+      </c>
+      <c r="Y73" s="58">
+        <f t="shared" si="153"/>
+        <v>0.12930311404774883</v>
+      </c>
+      <c r="Z73" s="58"/>
+      <c r="AA73" s="58">
+        <f t="shared" ref="AA73:AA77" si="154">R73/SUM($K73:$Q73)</f>
+        <v>1</v>
+      </c>
+      <c r="AB73" s="58">
+        <f t="shared" ref="AB73:AH77" si="155">K73/SUM($K73:$P73)</f>
+        <v>5.2487705940236877E-2</v>
+      </c>
+      <c r="AC73" s="58">
+        <f t="shared" si="155"/>
+        <v>0.63732735026582166</v>
+      </c>
+      <c r="AD73" s="58">
+        <f t="shared" si="155"/>
+        <v>0.16406389486698106</v>
+      </c>
+      <c r="AE73" s="58">
+        <f t="shared" si="155"/>
+        <v>8.4709304716629338E-2</v>
+      </c>
+      <c r="AF73" s="58">
+        <f t="shared" si="155"/>
+        <v>1.4458898629817427E-2</v>
+      </c>
+      <c r="AG73" s="58">
+        <f t="shared" si="155"/>
+        <v>4.6952845580513436E-2</v>
+      </c>
+      <c r="AH73" s="58">
+        <f t="shared" si="155"/>
+        <v>1.9847776700660999E-2</v>
+      </c>
+      <c r="AI73" s="59">
+        <f t="shared" ref="AI73:AI77" si="156">SUM($AB73:$AH73)</f>
+        <v>1.0198477767006608</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A74" s="49">
+        <v>2023</v>
+      </c>
+      <c r="B74" s="49">
+        <v>46</v>
+      </c>
+      <c r="C74" s="13">
+        <v>43</v>
+      </c>
+      <c r="D74" s="13">
+        <v>538</v>
+      </c>
+      <c r="E74" s="13">
+        <v>56</v>
+      </c>
+      <c r="F74" s="13">
+        <v>111</v>
+      </c>
+      <c r="G74" s="13">
+        <v>7</v>
+      </c>
+      <c r="H74" s="13">
+        <v>230</v>
+      </c>
+      <c r="I74" s="13">
+        <v>3</v>
+      </c>
+      <c r="J74" s="50">
+        <f t="shared" si="149"/>
+        <v>988</v>
+      </c>
+      <c r="K74" s="3">
+        <v>488.20609443355102</v>
+      </c>
+      <c r="L74" s="3">
+        <v>6911.6442358573122</v>
+      </c>
+      <c r="M74" s="3">
+        <v>1106.1559279110911</v>
+      </c>
+      <c r="N74" s="3">
+        <v>723.43127229628396</v>
+      </c>
+      <c r="O74" s="3">
+        <v>123.52499988059765</v>
+      </c>
+      <c r="P74" s="3">
+        <v>546.83503417580539</v>
+      </c>
+      <c r="Q74" s="3">
+        <v>136</v>
+      </c>
+      <c r="R74" s="38">
+        <f t="shared" si="150"/>
+        <v>10035.797564554641</v>
+      </c>
+      <c r="S74" s="39">
+        <f>(C74*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C74:H74)</f>
+        <v>11.04192748686437</v>
+      </c>
+      <c r="T74" s="58">
+        <f t="shared" si="151"/>
+        <v>4.8646466939293642E-2</v>
+      </c>
+      <c r="U74" s="58">
+        <f t="shared" si="152"/>
+        <v>0.68869904872020304</v>
+      </c>
+      <c r="V74" s="58">
+        <f t="shared" si="153"/>
+        <v>0.31490101030574424</v>
+      </c>
+      <c r="W74" s="58">
+        <f t="shared" si="153"/>
+        <v>0.20594676824909652</v>
+      </c>
+      <c r="X74" s="58">
+        <f t="shared" si="153"/>
+        <v>3.5165157351616738E-2</v>
+      </c>
+      <c r="Y74" s="58">
+        <f t="shared" si="153"/>
+        <v>0.15567326485129865</v>
+      </c>
+      <c r="Z74" s="58"/>
+      <c r="AA74" s="58">
+        <f t="shared" si="154"/>
+        <v>1</v>
+      </c>
+      <c r="AB74" s="58">
+        <f t="shared" si="155"/>
+        <v>4.9314755301818516E-2</v>
+      </c>
+      <c r="AC74" s="58">
+        <f t="shared" si="155"/>
+        <v>0.69816015840605161</v>
+      </c>
+      <c r="AD74" s="58">
+        <f t="shared" si="155"/>
+        <v>0.11173520677549868</v>
+      </c>
+      <c r="AE74" s="58">
+        <f t="shared" si="155"/>
+        <v>7.3075360135288661E-2</v>
+      </c>
+      <c r="AF74" s="58">
+        <f t="shared" si="155"/>
+        <v>1.2477527856010723E-2</v>
+      </c>
+      <c r="AG74" s="58">
+        <f t="shared" si="155"/>
+        <v>5.5236991525331826E-2</v>
+      </c>
+      <c r="AH74" s="58">
+        <f t="shared" si="155"/>
+        <v>1.3737654645276393E-2</v>
+      </c>
+      <c r="AI74" s="59">
+        <f t="shared" si="156"/>
+        <v>1.0137376546452763</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A75" s="49">
+        <v>2023</v>
+      </c>
+      <c r="B75" s="49">
+        <v>47</v>
+      </c>
+      <c r="C75" s="13">
+        <v>42</v>
+      </c>
+      <c r="D75" s="13">
+        <v>482</v>
+      </c>
+      <c r="E75" s="13">
+        <v>77</v>
+      </c>
+      <c r="F75" s="13">
+        <v>121</v>
+      </c>
+      <c r="G75" s="13">
+        <v>11</v>
+      </c>
+      <c r="H75" s="13">
+        <v>175</v>
+      </c>
+      <c r="I75" s="13">
+        <v>1</v>
+      </c>
+      <c r="J75" s="50">
+        <f t="shared" si="149"/>
+        <v>909</v>
+      </c>
+      <c r="K75" s="3">
+        <v>446.00001497325781</v>
+      </c>
+      <c r="L75" s="3">
+        <v>6295.4027893065813</v>
+      </c>
+      <c r="M75" s="3">
+        <v>1529.4642479564579</v>
+      </c>
+      <c r="N75" s="3">
+        <v>882.96433823468647</v>
+      </c>
+      <c r="O75" s="3">
+        <v>169.77217271693809</v>
+      </c>
+      <c r="P75" s="3">
+        <v>376.95850907960823</v>
+      </c>
+      <c r="Q75" s="3">
+        <v>35</v>
+      </c>
+      <c r="R75" s="38">
+        <f t="shared" si="150"/>
+        <v>9735.5620722675285</v>
+      </c>
+      <c r="S75" s="39">
+        <f>(C75*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C75:H75)</f>
+        <v>11.255394322236393</v>
+      </c>
+      <c r="T75" s="58">
+        <f t="shared" si="151"/>
+        <v>4.5811429444194286E-2</v>
+      </c>
+      <c r="U75" s="58">
+        <f t="shared" si="152"/>
+        <v>0.64663989018564261</v>
+      </c>
+      <c r="V75" s="58">
+        <f t="shared" si="153"/>
+        <v>0.43540862979194345</v>
+      </c>
+      <c r="W75" s="58">
+        <f t="shared" si="153"/>
+        <v>0.25136271944871236</v>
+      </c>
+      <c r="X75" s="58">
+        <f t="shared" si="153"/>
+        <v>4.8330825122750831E-2</v>
+      </c>
+      <c r="Y75" s="58">
+        <f t="shared" si="153"/>
+        <v>0.10731273264220735</v>
+      </c>
+      <c r="Z75" s="58"/>
+      <c r="AA75" s="58">
+        <f t="shared" si="154"/>
+        <v>1</v>
+      </c>
+      <c r="AB75" s="58">
+        <f t="shared" si="155"/>
+        <v>4.5976718838623365E-2</v>
+      </c>
+      <c r="AC75" s="58">
+        <f t="shared" si="155"/>
+        <v>0.64897299170985223</v>
+      </c>
+      <c r="AD75" s="58">
+        <f t="shared" si="155"/>
+        <v>0.15766759045117293</v>
+      </c>
+      <c r="AE75" s="58">
+        <f t="shared" si="155"/>
+        <v>9.1021977041820176E-2</v>
+      </c>
+      <c r="AF75" s="58">
+        <f t="shared" si="155"/>
+        <v>1.7501271725510793E-2</v>
+      </c>
+      <c r="AG75" s="58">
+        <f t="shared" si="155"/>
+        <v>3.8859450233020704E-2</v>
+      </c>
+      <c r="AH75" s="58">
+        <f t="shared" si="155"/>
+        <v>3.6080383527527567E-3</v>
+      </c>
+      <c r="AI75" s="59">
+        <f t="shared" si="156"/>
+        <v>1.003608038352753</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A76" s="49">
+        <v>2023</v>
+      </c>
+      <c r="B76" s="49">
+        <v>48</v>
+      </c>
+      <c r="C76" s="13">
+        <v>40</v>
+      </c>
+      <c r="D76" s="13">
+        <v>419</v>
+      </c>
+      <c r="E76" s="13">
+        <v>71</v>
+      </c>
+      <c r="F76" s="13">
+        <v>126</v>
+      </c>
+      <c r="G76" s="13">
+        <v>11</v>
+      </c>
+      <c r="H76" s="13">
+        <v>151</v>
+      </c>
+      <c r="I76" s="13">
+        <v>4</v>
+      </c>
+      <c r="J76" s="50">
+        <f t="shared" si="149"/>
+        <v>822</v>
+      </c>
+      <c r="K76" s="3">
+        <v>394.35456609878793</v>
+      </c>
+      <c r="L76" s="3">
+        <v>5169.0090640182416</v>
+      </c>
+      <c r="M76" s="3">
+        <v>1454.5380151166046</v>
+      </c>
+      <c r="N76" s="3">
+        <v>862.32824085601897</v>
+      </c>
+      <c r="O76" s="3">
+        <v>174.65499845086453</v>
+      </c>
+      <c r="P76" s="3">
+        <v>347.35886884377516</v>
+      </c>
+      <c r="Q76" s="3">
+        <v>97.419410664231847</v>
+      </c>
+      <c r="R76" s="38">
+        <f t="shared" si="150"/>
+        <v>8499.6631640485248</v>
+      </c>
+      <c r="S76" s="39">
+        <f>(C76*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C76:H76)</f>
+        <v>11.423440717089179</v>
+      </c>
+      <c r="T76" s="58">
+        <f t="shared" si="151"/>
+        <v>4.6396493424211246E-2</v>
+      </c>
+      <c r="U76" s="58">
+        <f t="shared" si="152"/>
+        <v>0.60814281275073023</v>
+      </c>
+      <c r="V76" s="58">
+        <f t="shared" si="153"/>
+        <v>0.41407859319915519</v>
+      </c>
+      <c r="W76" s="58">
+        <f t="shared" si="153"/>
+        <v>0.24548802515892826</v>
+      </c>
+      <c r="X76" s="58">
+        <f t="shared" si="153"/>
+        <v>4.9720870339670653E-2</v>
+      </c>
+      <c r="Y76" s="58">
+        <f t="shared" si="153"/>
+        <v>9.8886292589987532E-2</v>
+      </c>
+      <c r="Z76" s="58"/>
+      <c r="AA76" s="58">
+        <f t="shared" si="154"/>
+        <v>1</v>
+      </c>
+      <c r="AB76" s="58">
+        <f t="shared" si="155"/>
+        <v>4.693443533341294E-2</v>
+      </c>
+      <c r="AC76" s="58">
+        <f t="shared" si="155"/>
+        <v>0.61519389531352797</v>
+      </c>
+      <c r="AD76" s="58">
+        <f t="shared" si="155"/>
+        <v>0.1731130466824102</v>
+      </c>
+      <c r="AE76" s="58">
+        <f t="shared" si="155"/>
+        <v>0.10263070986350362</v>
+      </c>
+      <c r="AF76" s="58">
+        <f t="shared" si="155"/>
+        <v>2.0786709309702688E-2</v>
+      </c>
+      <c r="AG76" s="58">
+        <f t="shared" si="155"/>
+        <v>4.1341203497442504E-2</v>
+      </c>
+      <c r="AH76" s="58">
+        <f t="shared" si="155"/>
+        <v>1.1594451854005405E-2</v>
+      </c>
+      <c r="AI76" s="59">
+        <f t="shared" si="156"/>
+        <v>1.0115944518540054</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A77" s="49">
+        <v>2023</v>
+      </c>
+      <c r="B77" s="49">
+        <v>49</v>
+      </c>
+      <c r="C77" s="13">
+        <v>39</v>
+      </c>
+      <c r="D77" s="13">
+        <v>449</v>
+      </c>
+      <c r="E77" s="13">
+        <v>58</v>
+      </c>
+      <c r="F77" s="13">
+        <v>116</v>
+      </c>
+      <c r="G77" s="13">
+        <v>7</v>
+      </c>
+      <c r="H77" s="13">
+        <v>176</v>
+      </c>
+      <c r="I77" s="13">
+        <v>6</v>
+      </c>
+      <c r="J77" s="50">
+        <f t="shared" si="149"/>
+        <v>851</v>
+      </c>
+      <c r="K77" s="3">
+        <v>379.05395985218553</v>
+      </c>
+      <c r="L77" s="3">
+        <v>5637.4895128204225</v>
+      </c>
+      <c r="M77" s="3">
+        <v>1171.1360804265946</v>
+      </c>
+      <c r="N77" s="3">
+        <v>829.02434486168477</v>
+      </c>
+      <c r="O77" s="3">
+        <v>119.49999809265137</v>
+      </c>
+      <c r="P77" s="3">
+        <v>377.46436081187881</v>
+      </c>
+      <c r="Q77" s="3">
+        <v>273.40373616874427</v>
+      </c>
+      <c r="R77" s="38">
+        <f t="shared" si="150"/>
+        <v>8787.071993034162</v>
+      </c>
+      <c r="S77" s="39">
+        <f>(C77*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C77:H77)</f>
+        <v>11.293444063808437</v>
+      </c>
+      <c r="T77" s="58">
+        <f t="shared" si="151"/>
+        <v>4.3137686837285007E-2</v>
+      </c>
+      <c r="U77" s="58">
+        <f t="shared" si="152"/>
+        <v>0.64156632804300107</v>
+      </c>
+      <c r="V77" s="58">
+        <f t="shared" si="153"/>
+        <v>0.33339959188962209</v>
+      </c>
+      <c r="W77" s="58">
+        <f t="shared" si="153"/>
+        <v>0.23600705576654055</v>
+      </c>
+      <c r="X77" s="58">
+        <f t="shared" si="153"/>
+        <v>3.4019317874988644E-2</v>
+      </c>
+      <c r="Y77" s="58">
+        <f t="shared" si="153"/>
+        <v>0.10745673876063744</v>
+      </c>
+      <c r="Z77" s="58"/>
+      <c r="AA77" s="58">
+        <f t="shared" si="154"/>
+        <v>1</v>
+      </c>
+      <c r="AB77" s="58">
+        <f t="shared" si="155"/>
+        <v>4.4522989199927608E-2</v>
+      </c>
+      <c r="AC77" s="58">
+        <f t="shared" si="155"/>
+        <v>0.66216927213182797</v>
+      </c>
+      <c r="AD77" s="58">
+        <f t="shared" si="155"/>
+        <v>0.13755951548642867</v>
+      </c>
+      <c r="AE77" s="58">
+        <f t="shared" si="155"/>
+        <v>9.7375692809402101E-2</v>
+      </c>
+      <c r="AF77" s="58">
+        <f t="shared" si="155"/>
+        <v>1.4036252586690423E-2</v>
+      </c>
+      <c r="AG77" s="58">
+        <f t="shared" si="155"/>
+        <v>4.4336277785723181E-2</v>
+      </c>
+      <c r="AH77" s="58">
+        <f t="shared" si="155"/>
+        <v>3.2113505943606818E-2</v>
+      </c>
+      <c r="AI77" s="59">
+        <f t="shared" si="156"/>
+        <v>1.0321135059436066</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16202,10 +17258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:A72"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18660,6 +19716,244 @@
         <v>15.176211322772104</v>
       </c>
     </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B73" s="52">
+        <v>45</v>
+      </c>
+      <c r="C73" s="13">
+        <v>0</v>
+      </c>
+      <c r="D73" s="13">
+        <v>8</v>
+      </c>
+      <c r="E73" s="13">
+        <v>12</v>
+      </c>
+      <c r="F73" s="13">
+        <v>10</v>
+      </c>
+      <c r="G73" s="13">
+        <v>5</v>
+      </c>
+      <c r="H73" s="13">
+        <v>3</v>
+      </c>
+      <c r="I73">
+        <f t="shared" ref="I73:I79" si="10">SUM(C73:H73)</f>
+        <v>38</v>
+      </c>
+      <c r="J73" s="11">
+        <f>(C73*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E73*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C73:H73)</f>
+        <v>16.690074349799939</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B74" s="52">
+        <v>46</v>
+      </c>
+      <c r="C74" s="13">
+        <v>0</v>
+      </c>
+      <c r="D74" s="13">
+        <v>27</v>
+      </c>
+      <c r="E74" s="13">
+        <v>5</v>
+      </c>
+      <c r="F74" s="13">
+        <v>2</v>
+      </c>
+      <c r="G74" s="13">
+        <v>6</v>
+      </c>
+      <c r="H74" s="13">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="J74" s="11">
+        <f>(C74*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E74*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C74:H74)</f>
+        <v>15.830891812865499</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B75" s="52">
+        <v>47</v>
+      </c>
+      <c r="C75" s="13">
+        <v>0</v>
+      </c>
+      <c r="D75" s="13">
+        <v>20</v>
+      </c>
+      <c r="E75" s="13">
+        <v>1</v>
+      </c>
+      <c r="F75" s="13">
+        <v>4</v>
+      </c>
+      <c r="G75" s="13">
+        <v>10</v>
+      </c>
+      <c r="H75" s="13">
+        <v>3</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="10"/>
+        <v>38</v>
+      </c>
+      <c r="J75" s="11">
+        <f>(C75*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E75*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C75:H75)</f>
+        <v>15.258149142043706</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B76" s="52">
+        <v>48</v>
+      </c>
+      <c r="C76" s="13">
+        <v>0</v>
+      </c>
+      <c r="D76" s="13">
+        <v>30</v>
+      </c>
+      <c r="E76" s="13">
+        <v>1</v>
+      </c>
+      <c r="F76" s="13">
+        <v>4</v>
+      </c>
+      <c r="G76" s="13">
+        <v>7</v>
+      </c>
+      <c r="H76" s="13">
+        <v>3</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="J76" s="11">
+        <f>(C76*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E76*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C76:H76)</f>
+        <v>14.714600795971414</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B77" s="52">
+        <v>49</v>
+      </c>
+      <c r="C77" s="13">
+        <v>0</v>
+      </c>
+      <c r="D77" s="13">
+        <v>26</v>
+      </c>
+      <c r="E77" s="13">
+        <v>3</v>
+      </c>
+      <c r="F77" s="13">
+        <v>4</v>
+      </c>
+      <c r="G77" s="13">
+        <v>11</v>
+      </c>
+      <c r="H77" s="13">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="10"/>
+        <v>46</v>
+      </c>
+      <c r="J77" s="11">
+        <f>(C77*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E77*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C77:H77)</f>
+        <v>15.666122393846935</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B78" s="52">
+        <v>50</v>
+      </c>
+      <c r="C78" s="13">
+        <v>0</v>
+      </c>
+      <c r="D78" s="13">
+        <v>41</v>
+      </c>
+      <c r="E78" s="13">
+        <v>4</v>
+      </c>
+      <c r="F78" s="13">
+        <v>0</v>
+      </c>
+      <c r="G78" s="13">
+        <v>9</v>
+      </c>
+      <c r="H78" s="13">
+        <v>3</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="10"/>
+        <v>57</v>
+      </c>
+      <c r="J78" s="11">
+        <f>(C78*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D78*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E78*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F78*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G78*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H78*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C78:H78)</f>
+        <v>14.741700330871039</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="52">
+        <v>2023</v>
+      </c>
+      <c r="B79" s="52">
+        <v>51</v>
+      </c>
+      <c r="C79" s="13">
+        <v>0</v>
+      </c>
+      <c r="D79" s="13">
+        <v>31</v>
+      </c>
+      <c r="E79" s="13">
+        <v>4</v>
+      </c>
+      <c r="F79" s="13">
+        <v>2</v>
+      </c>
+      <c r="G79" s="13">
+        <v>13</v>
+      </c>
+      <c r="H79" s="13">
+        <v>6</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="10"/>
+        <v>56</v>
+      </c>
+      <c r="J79" s="11">
+        <f>(C79*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D79*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E79*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F79*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G79*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H79*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C79:H79)</f>
+        <v>14.663393509816206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -18670,10 +19964,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6335AA81-92E1-4191-98F5-D9E75D89EE86}">
-  <dimension ref="A1:J287"/>
+  <dimension ref="A1:J322"/>
   <sheetViews>
-    <sheetView topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="I288" sqref="I288"/>
+    <sheetView topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="H323" sqref="H323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28135,6 +29429,1161 @@
         <v>9</v>
       </c>
     </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>2023</v>
+      </c>
+      <c r="B288">
+        <v>45</v>
+      </c>
+      <c r="C288" t="s">
+        <v>57</v>
+      </c>
+      <c r="D288">
+        <v>0</v>
+      </c>
+      <c r="E288">
+        <v>2</v>
+      </c>
+      <c r="F288">
+        <v>0</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>2</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288">
+        <f t="shared" ref="J288:J292" si="55">SUM(D288:I288)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>2023</v>
+      </c>
+      <c r="B289">
+        <v>45</v>
+      </c>
+      <c r="C289" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <v>6</v>
+      </c>
+      <c r="F289">
+        <v>0</v>
+      </c>
+      <c r="G289">
+        <v>4</v>
+      </c>
+      <c r="H289">
+        <v>2</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289">
+        <f t="shared" si="55"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>2023</v>
+      </c>
+      <c r="B290">
+        <v>45</v>
+      </c>
+      <c r="C290" t="s">
+        <v>60</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="E290">
+        <v>0</v>
+      </c>
+      <c r="F290">
+        <v>12</v>
+      </c>
+      <c r="G290">
+        <v>1</v>
+      </c>
+      <c r="H290">
+        <v>6</v>
+      </c>
+      <c r="I290">
+        <v>3</v>
+      </c>
+      <c r="J290">
+        <f t="shared" si="55"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>2023</v>
+      </c>
+      <c r="B291">
+        <v>45</v>
+      </c>
+      <c r="C291" t="s">
+        <v>69</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291">
+        <v>0</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>2023</v>
+      </c>
+      <c r="B292">
+        <v>45</v>
+      </c>
+      <c r="C292" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292">
+        <v>0</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+      <c r="H292">
+        <v>0</v>
+      </c>
+      <c r="I292">
+        <v>0</v>
+      </c>
+      <c r="J292">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>2023</v>
+      </c>
+      <c r="B293">
+        <v>46</v>
+      </c>
+      <c r="C293" t="s">
+        <v>57</v>
+      </c>
+      <c r="D293">
+        <v>0</v>
+      </c>
+      <c r="E293">
+        <v>2</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293">
+        <v>0</v>
+      </c>
+      <c r="J293">
+        <f t="shared" ref="J293:J297" si="56">SUM(D293:I293)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>2023</v>
+      </c>
+      <c r="B294">
+        <v>46</v>
+      </c>
+      <c r="C294" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D294">
+        <v>0</v>
+      </c>
+      <c r="E294">
+        <v>8</v>
+      </c>
+      <c r="F294">
+        <v>2</v>
+      </c>
+      <c r="G294">
+        <v>1</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294">
+        <f t="shared" si="56"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>2023</v>
+      </c>
+      <c r="B295">
+        <v>46</v>
+      </c>
+      <c r="C295" t="s">
+        <v>60</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295">
+        <v>8</v>
+      </c>
+      <c r="F295">
+        <v>1</v>
+      </c>
+      <c r="G295">
+        <v>4</v>
+      </c>
+      <c r="H295">
+        <v>2</v>
+      </c>
+      <c r="I295">
+        <v>0</v>
+      </c>
+      <c r="J295">
+        <f t="shared" si="56"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>2023</v>
+      </c>
+      <c r="B296">
+        <v>46</v>
+      </c>
+      <c r="C296" t="s">
+        <v>69</v>
+      </c>
+      <c r="D296">
+        <v>0</v>
+      </c>
+      <c r="E296">
+        <v>5</v>
+      </c>
+      <c r="F296">
+        <v>2</v>
+      </c>
+      <c r="G296">
+        <v>1</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296">
+        <v>0</v>
+      </c>
+      <c r="J296">
+        <f t="shared" si="56"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>2023</v>
+      </c>
+      <c r="B297">
+        <v>46</v>
+      </c>
+      <c r="C297" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297">
+        <v>4</v>
+      </c>
+      <c r="F297">
+        <v>0</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+      <c r="H297">
+        <v>0</v>
+      </c>
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="J297">
+        <f t="shared" si="56"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>2023</v>
+      </c>
+      <c r="B298">
+        <v>47</v>
+      </c>
+      <c r="C298" t="s">
+        <v>57</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298">
+        <v>2</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+      <c r="H298">
+        <v>2</v>
+      </c>
+      <c r="I298">
+        <v>0</v>
+      </c>
+      <c r="J298">
+        <f t="shared" ref="J298:J302" si="57">SUM(D298:I298)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>2023</v>
+      </c>
+      <c r="B299">
+        <v>47</v>
+      </c>
+      <c r="C299" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299">
+        <v>6</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+      <c r="G299">
+        <v>4</v>
+      </c>
+      <c r="H299">
+        <v>2</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299">
+        <f t="shared" si="57"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>2023</v>
+      </c>
+      <c r="B300">
+        <v>47</v>
+      </c>
+      <c r="C300" t="s">
+        <v>60</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300">
+        <v>12</v>
+      </c>
+      <c r="F300">
+        <v>1</v>
+      </c>
+      <c r="G300">
+        <v>6</v>
+      </c>
+      <c r="H300">
+        <v>0</v>
+      </c>
+      <c r="I300">
+        <v>3</v>
+      </c>
+      <c r="J300">
+        <f t="shared" si="57"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>2023</v>
+      </c>
+      <c r="B301">
+        <v>47</v>
+      </c>
+      <c r="C301" t="s">
+        <v>69</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301">
+        <v>0</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+      <c r="H301">
+        <v>0</v>
+      </c>
+      <c r="I301">
+        <v>0</v>
+      </c>
+      <c r="J301">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>2023</v>
+      </c>
+      <c r="B302">
+        <v>47</v>
+      </c>
+      <c r="C302" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>0</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+      <c r="G302">
+        <v>0</v>
+      </c>
+      <c r="H302">
+        <v>0</v>
+      </c>
+      <c r="I302">
+        <v>0</v>
+      </c>
+      <c r="J302">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>2023</v>
+      </c>
+      <c r="B303">
+        <v>48</v>
+      </c>
+      <c r="C303" t="s">
+        <v>57</v>
+      </c>
+      <c r="D303">
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>2</v>
+      </c>
+      <c r="F303">
+        <v>1</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+      <c r="H303">
+        <v>0</v>
+      </c>
+      <c r="I303">
+        <v>0</v>
+      </c>
+      <c r="J303">
+        <f t="shared" ref="J303:J307" si="58">SUM(D303:I303)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>2023</v>
+      </c>
+      <c r="B304">
+        <v>48</v>
+      </c>
+      <c r="C304" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D304">
+        <v>0</v>
+      </c>
+      <c r="E304">
+        <v>6</v>
+      </c>
+      <c r="F304">
+        <v>0</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+      <c r="H304">
+        <v>0</v>
+      </c>
+      <c r="I304">
+        <v>0</v>
+      </c>
+      <c r="J304">
+        <f t="shared" si="58"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>2023</v>
+      </c>
+      <c r="B305">
+        <v>48</v>
+      </c>
+      <c r="C305" t="s">
+        <v>60</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+      <c r="E305">
+        <v>16</v>
+      </c>
+      <c r="F305">
+        <v>0</v>
+      </c>
+      <c r="G305">
+        <v>5</v>
+      </c>
+      <c r="H305">
+        <v>2</v>
+      </c>
+      <c r="I305">
+        <v>3</v>
+      </c>
+      <c r="J305">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>2023</v>
+      </c>
+      <c r="B306">
+        <v>48</v>
+      </c>
+      <c r="C306" t="s">
+        <v>69</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+      <c r="E306">
+        <v>3</v>
+      </c>
+      <c r="F306">
+        <v>0</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+      <c r="H306">
+        <v>2</v>
+      </c>
+      <c r="I306">
+        <v>0</v>
+      </c>
+      <c r="J306">
+        <f t="shared" si="58"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>2023</v>
+      </c>
+      <c r="B307">
+        <v>48</v>
+      </c>
+      <c r="C307" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307">
+        <v>3</v>
+      </c>
+      <c r="F307">
+        <v>0</v>
+      </c>
+      <c r="G307">
+        <v>2</v>
+      </c>
+      <c r="H307">
+        <v>0</v>
+      </c>
+      <c r="I307">
+        <v>0</v>
+      </c>
+      <c r="J307">
+        <f t="shared" si="58"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>2023</v>
+      </c>
+      <c r="B308">
+        <v>49</v>
+      </c>
+      <c r="C308" t="s">
+        <v>57</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+      <c r="E308">
+        <v>0</v>
+      </c>
+      <c r="F308">
+        <v>1</v>
+      </c>
+      <c r="G308">
+        <v>3</v>
+      </c>
+      <c r="H308">
+        <v>0</v>
+      </c>
+      <c r="I308">
+        <v>1</v>
+      </c>
+      <c r="J308">
+        <f t="shared" ref="J308:J312" si="59">SUM(D308:I308)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>2023</v>
+      </c>
+      <c r="B309">
+        <v>49</v>
+      </c>
+      <c r="C309" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+      <c r="E309">
+        <v>12</v>
+      </c>
+      <c r="F309">
+        <v>1</v>
+      </c>
+      <c r="G309">
+        <v>2</v>
+      </c>
+      <c r="H309">
+        <v>1</v>
+      </c>
+      <c r="I309">
+        <v>0</v>
+      </c>
+      <c r="J309">
+        <f t="shared" si="59"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>2023</v>
+      </c>
+      <c r="B310">
+        <v>49</v>
+      </c>
+      <c r="C310" t="s">
+        <v>60</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>11</v>
+      </c>
+      <c r="F310">
+        <v>1</v>
+      </c>
+      <c r="G310">
+        <v>5</v>
+      </c>
+      <c r="H310">
+        <v>1</v>
+      </c>
+      <c r="I310">
+        <v>1</v>
+      </c>
+      <c r="J310">
+        <f t="shared" si="59"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>2023</v>
+      </c>
+      <c r="B311">
+        <v>49</v>
+      </c>
+      <c r="C311" t="s">
+        <v>69</v>
+      </c>
+      <c r="D311">
+        <v>0</v>
+      </c>
+      <c r="E311">
+        <v>3</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+      <c r="G311">
+        <v>1</v>
+      </c>
+      <c r="H311">
+        <v>2</v>
+      </c>
+      <c r="I311">
+        <v>0</v>
+      </c>
+      <c r="J311">
+        <f t="shared" si="59"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>2023</v>
+      </c>
+      <c r="B312">
+        <v>49</v>
+      </c>
+      <c r="C312" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D312">
+        <v>0</v>
+      </c>
+      <c r="E312">
+        <v>0</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>0</v>
+      </c>
+      <c r="J312">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>2023</v>
+      </c>
+      <c r="B313">
+        <v>50</v>
+      </c>
+      <c r="C313" t="s">
+        <v>57</v>
+      </c>
+      <c r="D313">
+        <v>0</v>
+      </c>
+      <c r="E313">
+        <v>6</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313">
+        <f t="shared" ref="J313:J317" si="60">SUM(D313:I313)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>2023</v>
+      </c>
+      <c r="B314">
+        <v>50</v>
+      </c>
+      <c r="C314" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D314">
+        <v>0</v>
+      </c>
+      <c r="E314">
+        <v>19</v>
+      </c>
+      <c r="F314">
+        <v>1</v>
+      </c>
+      <c r="G314">
+        <v>4</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+      <c r="I314">
+        <v>0</v>
+      </c>
+      <c r="J314">
+        <f t="shared" si="60"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>2023</v>
+      </c>
+      <c r="B315">
+        <v>50</v>
+      </c>
+      <c r="C315" t="s">
+        <v>60</v>
+      </c>
+      <c r="D315">
+        <v>0</v>
+      </c>
+      <c r="E315">
+        <v>9</v>
+      </c>
+      <c r="F315">
+        <v>3</v>
+      </c>
+      <c r="G315">
+        <v>4</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+      <c r="I315">
+        <v>3</v>
+      </c>
+      <c r="J315">
+        <f t="shared" si="60"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>2023</v>
+      </c>
+      <c r="B316">
+        <v>50</v>
+      </c>
+      <c r="C316" t="s">
+        <v>69</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316">
+        <v>2</v>
+      </c>
+      <c r="F316">
+        <v>0</v>
+      </c>
+      <c r="G316">
+        <v>1</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+      <c r="I316">
+        <v>0</v>
+      </c>
+      <c r="J316">
+        <f t="shared" si="60"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>2023</v>
+      </c>
+      <c r="B317">
+        <v>50</v>
+      </c>
+      <c r="C317" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+      <c r="E317">
+        <v>5</v>
+      </c>
+      <c r="F317">
+        <v>0</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+      <c r="I317">
+        <v>0</v>
+      </c>
+      <c r="J317">
+        <f t="shared" si="60"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>2023</v>
+      </c>
+      <c r="B318">
+        <v>51</v>
+      </c>
+      <c r="C318" t="s">
+        <v>57</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>2</v>
+      </c>
+      <c r="F318">
+        <v>0</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+      <c r="H318">
+        <v>1</v>
+      </c>
+      <c r="I318">
+        <v>0</v>
+      </c>
+      <c r="J318">
+        <f t="shared" ref="J318:J322" si="61">SUM(D318:I318)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>2023</v>
+      </c>
+      <c r="B319">
+        <v>51</v>
+      </c>
+      <c r="C319" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319">
+        <v>16</v>
+      </c>
+      <c r="F319">
+        <v>0</v>
+      </c>
+      <c r="G319">
+        <v>10</v>
+      </c>
+      <c r="H319">
+        <v>0</v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319">
+        <f t="shared" si="61"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>2023</v>
+      </c>
+      <c r="B320">
+        <v>51</v>
+      </c>
+      <c r="C320" t="s">
+        <v>60</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>8</v>
+      </c>
+      <c r="F320">
+        <v>3</v>
+      </c>
+      <c r="G320">
+        <v>1</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+      <c r="I320">
+        <v>4</v>
+      </c>
+      <c r="J320">
+        <f t="shared" si="61"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>2023</v>
+      </c>
+      <c r="B321">
+        <v>51</v>
+      </c>
+      <c r="C321" t="s">
+        <v>69</v>
+      </c>
+      <c r="D321">
+        <v>0</v>
+      </c>
+      <c r="E321">
+        <v>3</v>
+      </c>
+      <c r="F321">
+        <v>1</v>
+      </c>
+      <c r="G321">
+        <v>2</v>
+      </c>
+      <c r="H321">
+        <v>1</v>
+      </c>
+      <c r="I321">
+        <v>1</v>
+      </c>
+      <c r="J321">
+        <f t="shared" si="61"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>2023</v>
+      </c>
+      <c r="B322">
+        <v>51</v>
+      </c>
+      <c r="C322" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322">
+        <v>2</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+      <c r="H322">
+        <v>0</v>
+      </c>
+      <c r="I322">
+        <v>0</v>
+      </c>
+      <c r="J322">
+        <f t="shared" si="61"/>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -28145,10 +30594,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EB2B5E-69B9-4E17-A8DC-DBA424D12F80}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:G45"/>
+      <selection activeCell="B46" sqref="B46:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29157,26 +31606,187 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="12">
+        <v>45</v>
+      </c>
+      <c r="B46" s="13">
+        <v>0</v>
+      </c>
+      <c r="C46" s="13">
+        <v>8</v>
+      </c>
+      <c r="D46" s="13">
+        <v>12</v>
+      </c>
+      <c r="E46" s="13">
+        <v>10</v>
+      </c>
+      <c r="F46" s="13">
+        <v>5</v>
+      </c>
+      <c r="G46" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="12">
+        <v>46</v>
+      </c>
+      <c r="B47" s="13">
+        <v>0</v>
+      </c>
+      <c r="C47" s="13">
+        <v>27</v>
+      </c>
+      <c r="D47" s="13">
+        <v>5</v>
+      </c>
+      <c r="E47" s="13">
+        <v>2</v>
+      </c>
+      <c r="F47" s="13">
+        <v>6</v>
+      </c>
+      <c r="G47" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="12">
+        <v>47</v>
+      </c>
+      <c r="B48" s="13">
+        <v>0</v>
+      </c>
+      <c r="C48" s="13">
+        <v>20</v>
+      </c>
+      <c r="D48" s="13">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13">
+        <v>4</v>
+      </c>
+      <c r="F48" s="13">
+        <v>10</v>
+      </c>
+      <c r="G48" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="12">
+        <v>48</v>
+      </c>
+      <c r="B49" s="13">
+        <v>0</v>
+      </c>
+      <c r="C49" s="13">
+        <v>30</v>
+      </c>
+      <c r="D49" s="13">
+        <v>1</v>
+      </c>
+      <c r="E49" s="13">
+        <v>4</v>
+      </c>
+      <c r="F49" s="13">
+        <v>7</v>
+      </c>
+      <c r="G49" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="12">
+        <v>49</v>
+      </c>
+      <c r="B50" s="13">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13">
+        <v>26</v>
+      </c>
+      <c r="D50" s="13">
+        <v>3</v>
+      </c>
+      <c r="E50" s="13">
+        <v>4</v>
+      </c>
+      <c r="F50" s="13">
+        <v>11</v>
+      </c>
+      <c r="G50" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="12">
+        <v>50</v>
+      </c>
+      <c r="B51" s="13">
+        <v>0</v>
+      </c>
+      <c r="C51" s="13">
+        <v>41</v>
+      </c>
+      <c r="D51" s="13">
+        <v>4</v>
+      </c>
+      <c r="E51" s="13">
+        <v>0</v>
+      </c>
+      <c r="F51" s="13">
+        <v>9</v>
+      </c>
+      <c r="G51" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="12">
+        <v>51</v>
+      </c>
+      <c r="B52" s="13">
+        <v>0</v>
+      </c>
+      <c r="C52" s="13">
+        <v>31</v>
+      </c>
+      <c r="D52" s="13">
+        <v>4</v>
+      </c>
+      <c r="E52" s="13">
+        <v>2</v>
+      </c>
+      <c r="F52" s="13">
+        <v>13</v>
+      </c>
+      <c r="G52" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B53" s="13">
         <v>52</v>
       </c>
-      <c r="C46" s="13">
-        <v>895</v>
-      </c>
-      <c r="D46" s="13">
-        <v>115</v>
-      </c>
-      <c r="E46" s="13">
-        <v>176</v>
-      </c>
-      <c r="F46" s="13">
-        <v>330</v>
-      </c>
-      <c r="G46" s="13">
-        <v>151</v>
+      <c r="C53" s="13">
+        <v>1078</v>
+      </c>
+      <c r="D53" s="13">
+        <v>145</v>
+      </c>
+      <c r="E53" s="13">
+        <v>202</v>
+      </c>
+      <c r="F53" s="13">
+        <v>391</v>
+      </c>
+      <c r="G53" s="13">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -29188,7 +31798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Encerrando projeto bônus e iniciando projeto nova operação
</commit_message>
<xml_diff>
--- a/BANDEJA DO PERIODO.xlsx
+++ b/BANDEJA DO PERIODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/980841a2e24dade8/Profissional/The Coffee/Operação/2.Gestão da Qualidade/Bandejas/Bandejas semanais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4064" documentId="13_ncr:4000b_{D3240E66-DB17-44F6-81B1-0D6B85E22F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3952D05A-2D44-4AFF-8C9E-0928180011D6}"/>
+  <xr:revisionPtr revIDLastSave="4282" documentId="13_ncr:4000b_{D3240E66-DB17-44F6-81B1-0D6B85E22F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B418FE18-42CE-4AD1-9C60-76E8AFFFDE2A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="período" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="13" r:id="rId8"/>
+    <pivotCache cacheId="11" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="83">
   <si>
     <t xml:space="preserve">               New / App / Cold</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>Talita</t>
+  </si>
+  <si>
+    <t>Ticket médio de produtos disponíveis (BR-C/fev-24)</t>
   </si>
 </sst>
 </file>
@@ -1812,9 +1815,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gabriel Bezerra de Melo Silva" refreshedDate="45336.922307291665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="356" xr:uid="{9B5733B9-D351-4D08-9F8A-CB6331F2432F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gabriel Bezerra de Melo Silva" refreshedDate="45371.706183912036" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="381" xr:uid="{9B5733B9-D351-4D08-9F8A-CB6331F2432F}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J357" sheet="baristas"/>
+    <worksheetSource ref="A1:J382" sheet="baristas"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Ano" numFmtId="0">
@@ -1825,7 +1828,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Semana" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="53" count="52">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="53" count="53">
         <n v="41"/>
         <n v="42"/>
         <n v="43"/>
@@ -1877,6 +1880,7 @@
         <n v="38"/>
         <n v="39"/>
         <n v="40"/>
+        <n v="7"/>
         <n v="33" u="1"/>
       </sharedItems>
     </cacheField>
@@ -2783,7 +2787,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="356">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="381">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -7056,12 +7060,312 @@
     <n v="0"/>
     <n v="8"/>
   </r>
+  <r>
+    <x v="2"/>
+    <x v="51"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="51"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="15"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="51"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="51"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="1"/>
+    <n v="9"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="51"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="19"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="19"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="13"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="19"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="19"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="19"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="7"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="21"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="21"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="21"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="21"/>
+    <s v="Evelyn"/>
+    <n v="1"/>
+    <n v="12"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="3"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="21"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <s v="Jéssica"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <s v="Carolina"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <s v="Iasmym"/>
+    <n v="0"/>
+    <n v="7"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <s v="Evelyn"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <s v="Talita"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{993A75B1-F664-4E54-94B9-642F255C2CD9}" name="Tabela dinâmica5" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{993A75B1-F664-4E54-94B9-642F255C2CD9}" name="Tabela dinâmica5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" showAll="0">
       <items count="4">
@@ -7072,13 +7376,14 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="53">
+      <items count="54">
         <item x="13"/>
         <item x="14"/>
         <item x="15"/>
         <item x="16"/>
         <item x="17"/>
         <item x="18"/>
+        <item x="51"/>
         <item x="19"/>
         <item x="20"/>
         <item x="21"/>
@@ -7104,7 +7409,7 @@
         <item x="41"/>
         <item x="42"/>
         <item x="43"/>
-        <item m="1" x="51"/>
+        <item m="1" x="52"/>
         <item x="44"/>
         <item x="45"/>
         <item x="46"/>
@@ -7140,7 +7445,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="12">
     <i>
       <x/>
     </i>
@@ -7158,6 +7463,21 @@
     </i>
     <i>
       <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i t="grand">
       <x/>
@@ -7398,8 +7718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}" name="Tabela1" displayName="Tabela1" ref="A1:AI86" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" dataCellStyle="Porcentagem">
-  <autoFilter ref="A1:AI86" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}" name="Tabela1" displayName="Tabela1" ref="A1:AI89" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" dataCellStyle="Porcentagem">
+  <autoFilter ref="A1:AI89" xr:uid="{5B5D9E64-24ED-42BB-9763-8BC754E6493A}">
     <filterColumn colId="0">
       <filters>
         <filter val="2023"/>
@@ -7430,7 +7750,7 @@
       <calculatedColumnFormula>SUM(K2:Q2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{BDAED799-A45F-4E6C-A49B-F47A77327A56}" name="Ticket período" dataDxfId="22">
-      <calculatedColumnFormula>(C2*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C2:H2)</calculatedColumnFormula>
+      <calculatedColumnFormula>(C2*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C2:H2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{180F3C0A-C5B0-4129-AF46-1A6F46AB2FAC}" name="A$%  total" dataDxfId="21" dataCellStyle="Porcentagem">
       <calculatedColumnFormula>$K2/SUM($K2:$Q2)</calculatedColumnFormula>
@@ -7484,8 +7804,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}" name="Tabela2" displayName="Tabela2" ref="A1:J86" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:J86" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}" name="Tabela2" displayName="Tabela2" ref="A1:J91" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:J91" xr:uid="{8C617F03-4756-4E7E-89E1-3D05D07FEFA9}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{B3A7EC93-D052-476E-A7D0-7F9FEE82E6EB}" name="Ano" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{8907E03F-0276-4E6E-BA76-03A5F7E7ABA8}" name="Semana" dataDxfId="3"/>
@@ -7499,7 +7819,7 @@
       <calculatedColumnFormula>SUM(C2:H2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{C514D4B9-0A71-4B2C-A024-55D260D421F2}" name="Ticket Recomendado" dataDxfId="2">
-      <calculatedColumnFormula>(C2*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E2*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C2:H2)</calculatedColumnFormula>
+      <calculatedColumnFormula>(C2*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E2*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C2:H2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7507,8 +7827,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}" name="Tabela3" displayName="Tabela3" ref="A1:J357" totalsRowShown="0">
-  <autoFilter ref="A1:J357" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}" name="Tabela3" displayName="Tabela3" ref="A1:J382" totalsRowShown="0">
+  <autoFilter ref="A1:J382" xr:uid="{703EDD0E-C0B1-4373-BA4B-5824553F7E4F}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{19C2ECCC-C5CA-4CBA-9A19-FCC8487A8CC6}" name="Ano"/>
     <tableColumn id="1" xr3:uid="{42E434D7-D8A5-4430-8FC7-28848FD6B96A}" name="Semana"/>
@@ -7528,9 +7848,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7568,7 +7888,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7674,7 +7994,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7816,7 +8136,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7835,13 +8155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AK86"/>
+  <dimension ref="A1:AK89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8038,7 +8358,7 @@
         <v>3512.7100000000005</v>
       </c>
       <c r="S2" s="15">
-        <f>(C2*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C2:H2)</f>
+        <f>(C2*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C2:H2)</f>
         <v>8.8622325581395351</v>
       </c>
       <c r="T2" s="20">
@@ -8165,7 +8485,7 @@
         <v>8752.4035000000003</v>
       </c>
       <c r="S3" s="15">
-        <f>(C3*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D3*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F3*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G3*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H3*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C3:H3)</f>
+        <f>(C3*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D3*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+F3*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G3*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H3*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C3:H3)</f>
         <v>8.8726769242401335</v>
       </c>
       <c r="T3" s="20">
@@ -8292,7 +8612,7 @@
         <v>7576.3340000000007</v>
       </c>
       <c r="S4" s="15">
-        <f>(C4*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D4*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F4*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G4*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H4*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C4:H4)</f>
+        <f>(C4*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D4*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+F4*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G4*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H4*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C4:H4)</f>
         <v>8.8366614860695272</v>
       </c>
       <c r="T4" s="20">
@@ -8419,7 +8739,7 @@
         <v>7588.371000000001</v>
       </c>
       <c r="S5" s="15">
-        <f>(C5*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D5*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F5*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G5*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H5*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C5:H5)</f>
+        <f>(C5*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D5*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+F5*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G5*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H5*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C5:H5)</f>
         <v>8.6117242620197807</v>
       </c>
       <c r="T5" s="20">
@@ -8546,7 +8866,7 @@
         <v>8832.9599999999991</v>
       </c>
       <c r="S6" s="15">
-        <f>(C6*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D6*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F6*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G6*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H6*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C6:H6)</f>
+        <f>(C6*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D6*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+F6*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G6*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H6*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C6:H6)</f>
         <v>8.7192880494006548</v>
       </c>
       <c r="T6" s="20">
@@ -8673,7 +8993,7 @@
         <v>8842.3524999999991</v>
       </c>
       <c r="S7" s="15">
-        <f>(C7*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D7*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F7*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G7*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H7*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C7:H7)</f>
+        <f>(C7*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D7*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F7*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G7*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H7*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C7:H7)</f>
         <v>10.839957911075956</v>
       </c>
       <c r="T7" s="20">
@@ -8800,7 +9120,7 @@
         <v>8028.5713749999995</v>
       </c>
       <c r="S8" s="18">
-        <f>(C8*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D8*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F8*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G8*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H8*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C8:H8)</f>
+        <f>(C8*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D8*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F8*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G8*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H8*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C8:H8)</f>
         <v>10.661622027750902</v>
       </c>
       <c r="T8" s="17">
@@ -8927,7 +9247,7 @@
         <v>7123.9099999999989</v>
       </c>
       <c r="S9" s="18">
-        <f>(C9*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D9*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F9*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G9*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H9*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C9:H9)</f>
+        <f>(C9*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D9*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F9*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G9*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H9*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C9:H9)</f>
         <v>10.424412136536029</v>
       </c>
       <c r="T9" s="17">
@@ -9054,7 +9374,7 @@
         <v>7163.1399999999994</v>
       </c>
       <c r="S10" s="18">
-        <f>(C10*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D10*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F10*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G10*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H10*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C10:H10)</f>
+        <f>(C10*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D10*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F10*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G10*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H10*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C10:H10)</f>
         <v>10.520092838196286</v>
       </c>
       <c r="T10" s="17">
@@ -9181,7 +9501,7 @@
         <v>8679.25</v>
       </c>
       <c r="S11" s="18">
-        <f>(C11*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D11*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F11*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G11*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H11*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C11:H11)</f>
+        <f>(C11*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D11*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F11*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G11*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H11*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C11:H11)</f>
         <v>10.407404063205419</v>
       </c>
       <c r="T11" s="17">
@@ -9308,7 +9628,7 @@
         <v>8843.8100000000013</v>
       </c>
       <c r="S12" s="18">
-        <f>(C12*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D12*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F12*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G12*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H12*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C12:H12)</f>
+        <f>(C12*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D12*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F12*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G12*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H12*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C12:H12)</f>
         <v>10.465438972162742</v>
       </c>
       <c r="T12" s="17">
@@ -9435,7 +9755,7 @@
         <v>8109.079999999999</v>
       </c>
       <c r="S13" s="18">
-        <f>(C13*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D13*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F13*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G13*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H13*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C13:H13)</f>
+        <f>(C13*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D13*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F13*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G13*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H13*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C13:H13)</f>
         <v>12.459713114754097</v>
       </c>
       <c r="T13" s="17">
@@ -9562,7 +9882,7 @@
         <v>7480.5499999999993</v>
       </c>
       <c r="S14" s="18">
-        <f>(C14*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D14*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F14*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G14*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H14*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C14:H14)</f>
+        <f>(C14*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D14*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F14*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G14*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H14*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C14:H14)</f>
         <v>10.825719557195571</v>
       </c>
       <c r="T14" s="17">
@@ -9689,7 +10009,7 @@
         <v>7309.7099999999991</v>
       </c>
       <c r="S15" s="18">
-        <f>(C15*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D15*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F15*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G15*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H15*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C15:H15)</f>
+        <f>(C15*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D15*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F15*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G15*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H15*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C15:H15)</f>
         <v>10.009850402761794</v>
       </c>
       <c r="T15" s="25">
@@ -9816,7 +10136,7 @@
         <v>8298.2999999999993</v>
       </c>
       <c r="S16" s="39">
-        <f>(C16*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D16*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F16*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G16*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H16*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C16:H16)</f>
+        <f>(C16*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D16*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F16*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G16*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H16*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C16:H16)</f>
         <v>10.226984978540772</v>
       </c>
       <c r="T16" s="40">
@@ -9943,7 +10263,7 @@
         <v>8024.23</v>
       </c>
       <c r="S17" s="39">
-        <f>(C17*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D17*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F17*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G17*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H17*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C17:H17)</f>
+        <f>(C17*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D17*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F17*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G17*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H17*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C17:H17)</f>
         <v>9.6995438996579253</v>
       </c>
       <c r="T17" s="41">
@@ -10070,7 +10390,7 @@
         <v>9023.0300000000007</v>
       </c>
       <c r="S18" s="39">
-        <f>(C18*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D18*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F18*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G18*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H18*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C18:H18)</f>
+        <f>(C18*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D18*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F18*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G18*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H18*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C18:H18)</f>
         <v>10.061565656565655</v>
       </c>
       <c r="T18" s="41">
@@ -10197,7 +10517,7 @@
         <v>7641.48</v>
       </c>
       <c r="S19" s="39">
-        <f>(C19*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D19*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F19*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G19*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H19*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C19:H19)</f>
+        <f>(C19*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D19*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F19*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G19*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H19*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C19:H19)</f>
         <v>10.159293413173653</v>
       </c>
       <c r="T19" s="41">
@@ -10324,7 +10644,7 @@
         <v>7183.23</v>
       </c>
       <c r="S20" s="39">
-        <f>(C20*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D20*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F20*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G20*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H20*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C20:H20)</f>
+        <f>(C20*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D20*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F20*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G20*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H20*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C20:H20)</f>
         <v>10.335182389937106</v>
       </c>
       <c r="T20" s="41">
@@ -10451,7 +10771,7 @@
         <v>7195.3899999999994</v>
       </c>
       <c r="S21" s="39">
-        <f>(C21*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D21*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F21*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G21*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H21*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C21:H21)</f>
+        <f>(C21*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D21*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F21*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G21*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H21*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C21:H21)</f>
         <v>10.498821081830791</v>
       </c>
       <c r="T21" s="41">
@@ -10578,7 +10898,7 @@
         <v>7026.1900000000005</v>
       </c>
       <c r="S22" s="39">
-        <f>(C22*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D22*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F22*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G22*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H22*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C22:H22)</f>
+        <f>(C22*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D22*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F22*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G22*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H22*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C22:H22)</f>
         <v>10.428664921465968</v>
       </c>
       <c r="T22" s="41">
@@ -10705,7 +11025,7 @@
         <v>7056.25</v>
       </c>
       <c r="S23" s="39">
-        <f>(C23*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D23*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F23*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G23*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H23*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C23:H23)</f>
+        <f>(C23*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D23*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F23*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G23*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H23*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C23:H23)</f>
         <v>9.9048575498575513</v>
       </c>
       <c r="T23" s="41">
@@ -10832,7 +11152,7 @@
         <v>7463.92</v>
       </c>
       <c r="S24" s="39">
-        <f>(C24*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D24*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F24*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G24*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H24*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C24:H24)</f>
+        <f>(C24*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D24*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F24*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G24*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H24*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C24:H24)</f>
         <v>9.8796805555555558</v>
       </c>
       <c r="T24" s="41">
@@ -10958,7 +11278,7 @@
         <v>8299.16</v>
       </c>
       <c r="S25" s="39">
-        <f>(C25*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D25*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F25*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G25*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H25*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C25:H25)</f>
+        <f>(C25*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D25*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F25*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G25*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H25*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C25:H25)</f>
         <v>9.8307116564417178</v>
       </c>
       <c r="T25" s="41">
@@ -11084,7 +11404,7 @@
         <v>9054.75</v>
       </c>
       <c r="S26" s="39">
-        <f>(C26*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D26*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F26*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G26*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H26*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C26:H26)</f>
+        <f>(C26*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D26*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F26*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G26*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H26*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C26:H26)</f>
         <v>9.713912087912087</v>
       </c>
       <c r="T26" s="41">
@@ -11210,7 +11530,7 @@
         <v>10110.799999999999</v>
       </c>
       <c r="S27" s="39">
-        <f>(C27*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D27*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F27*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G27*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H27*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C27:H27)</f>
+        <f>(C27*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D27*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F27*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G27*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H27*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C27:H27)</f>
         <v>9.6760650887573938</v>
       </c>
       <c r="T27" s="41">
@@ -11336,7 +11656,7 @@
         <v>9553.84</v>
       </c>
       <c r="S28" s="39">
-        <f>(C28*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D28*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+F28*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G28*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H28*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C28:H28)</f>
+        <f>(C28*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D28*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+F28*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G28*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H28*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C28:H28)</f>
         <v>9.5830785562632705</v>
       </c>
       <c r="T28" s="41">
@@ -11462,7 +11782,7 @@
         <v>8235.0299999999988</v>
       </c>
       <c r="S29" s="39">
-        <f>(C29*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D29*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F29*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G29*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H29*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C29:H29)</f>
+        <f>(C29*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D29*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F29*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G29*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H29*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C29:H29)</f>
         <v>9.911662790697676</v>
       </c>
       <c r="T29" s="58">
@@ -11588,7 +11908,7 @@
         <v>11390.290000000003</v>
       </c>
       <c r="S30" s="39">
-        <f>(C30*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D30*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F30*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G30*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H30*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C30:H30)</f>
+        <f>(C30*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D30*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F30*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G30*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H30*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C30:H30)</f>
         <v>9.998725314183126</v>
       </c>
       <c r="T30" s="58">
@@ -11714,7 +12034,7 @@
         <v>10407.419999999996</v>
       </c>
       <c r="S31" s="39">
-        <f>(C31*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D31*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F31*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G31*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H31*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C31:H31)</f>
+        <f>(C31*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D31*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F31*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G31*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H31*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C31:H31)</f>
         <v>9.8859042033235554</v>
       </c>
       <c r="T31" s="58">
@@ -11840,7 +12160,7 @@
         <v>9732.6700000000019</v>
       </c>
       <c r="S32" s="39">
-        <f>(C32*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D32*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F32*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G32*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H32*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C32:H32)</f>
+        <f>(C32*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D32*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F32*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G32*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H32*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C32:H32)</f>
         <v>10.255621734587251</v>
       </c>
       <c r="T32" s="58">
@@ -11966,7 +12286,7 @@
         <v>10076.489999999998</v>
       </c>
       <c r="S33" s="39">
-        <f>(C33*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D33*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F33*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G33*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H33*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C33:H33)</f>
+        <f>(C33*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D33*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F33*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G33*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H33*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C33:H33)</f>
         <v>9.8781038135593224</v>
       </c>
       <c r="T33" s="58">
@@ -12092,7 +12412,7 @@
         <v>10639.58</v>
       </c>
       <c r="S34" s="39">
-        <f>(C34*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D34*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F34*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G34*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H34*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C34:H34)</f>
+        <f>(C34*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D34*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F34*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G34*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H34*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C34:H34)</f>
         <v>9.9122084130019115</v>
       </c>
       <c r="T34" s="58">
@@ -12218,7 +12538,7 @@
         <v>9697.5400000000009</v>
       </c>
       <c r="S35" s="39">
-        <f>(C35*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D35*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F35*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G35*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H35*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C35:H35)</f>
+        <f>(C35*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D35*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F35*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G35*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H35*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C35:H35)</f>
         <v>9.7389738219895285</v>
       </c>
       <c r="T35" s="58">
@@ -12344,7 +12664,7 @@
         <v>8603.09</v>
       </c>
       <c r="S36" s="39">
-        <f>(C36*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D36*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F36*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G36*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H36*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C36:H36)</f>
+        <f>(C36*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D36*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F36*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G36*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H36*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C36:H36)</f>
         <v>9.9269195402298855</v>
       </c>
       <c r="T36" s="58">
@@ -12470,7 +12790,7 @@
         <v>10953.031950741113</v>
       </c>
       <c r="S37" s="39">
-        <f>(C37*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D37*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F37*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G37*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H37*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C37:H37)</f>
+        <f>(C37*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D37*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F37*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G37*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H37*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C37:H37)</f>
         <v>9.7660834088848585</v>
       </c>
       <c r="T37" s="58">
@@ -12596,7 +12916,7 @@
         <v>10905.046593417504</v>
       </c>
       <c r="S38" s="39">
-        <f>(C38*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D38*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F38*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G38*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H38*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C38:H38)</f>
+        <f>(C38*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D38*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F38*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G38*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H38*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C38:H38)</f>
         <v>9.6468636363636353</v>
       </c>
       <c r="T38" s="58">
@@ -12722,7 +13042,7 @@
         <v>9439.0643143017714</v>
       </c>
       <c r="S39" s="39">
-        <f>(C39*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D39*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F39*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G39*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H39*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C39:H39)</f>
+        <f>(C39*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D39*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F39*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G39*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H39*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C39:H39)</f>
         <v>10.100921501706484</v>
       </c>
       <c r="T39" s="58">
@@ -12848,7 +13168,7 @@
         <v>9760.0852854110308</v>
       </c>
       <c r="S40" s="39">
-        <f>(C40*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D40*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F40*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G40*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H40*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C40:H40)</f>
+        <f>(C40*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D40*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F40*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G40*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H40*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C40:H40)</f>
         <v>9.9437735849056619</v>
       </c>
       <c r="T40" s="58">
@@ -12974,7 +13294,7 @@
         <v>11181.229068587949</v>
       </c>
       <c r="S41" s="39">
-        <f>(C41*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D41*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F41*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G41*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H41*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C41:H41)</f>
+        <f>(C41*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D41*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F41*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G41*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H41*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C41:H41)</f>
         <v>10.190568181818183</v>
       </c>
       <c r="T41" s="58">
@@ -13100,7 +13420,7 @@
         <v>12219.470097158182</v>
       </c>
       <c r="S42" s="39">
-        <f>(C42*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D42*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F42*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G42*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H42*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C42:H42)</f>
+        <f>(C42*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D42*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F42*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G42*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H42*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C42:H42)</f>
         <v>9.8232074016962212</v>
       </c>
       <c r="T42" s="58">
@@ -13226,7 +13546,7 @@
         <v>11368.450103676121</v>
       </c>
       <c r="S43" s="39">
-        <f>(C43*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D43*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F43*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G43*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H43*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C43:H43)</f>
+        <f>(C43*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D43*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F43*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G43*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H43*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C43:H43)</f>
         <v>9.8622088006902473</v>
       </c>
       <c r="T43" s="58">
@@ -13352,7 +13672,7 @@
         <v>10735.600083143254</v>
       </c>
       <c r="S44" s="39">
-        <f>(C44*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D44*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F44*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G44*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H44*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C44:H44)</f>
+        <f>(C44*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D44*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F44*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G44*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H44*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C44:H44)</f>
         <v>9.7726173285198552</v>
       </c>
       <c r="T44" s="58">
@@ -13478,7 +13798,7 @@
         <v>10744.700070439605</v>
       </c>
       <c r="S45" s="39">
-        <f>(C45*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D45*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F45*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G45*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H45*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C45:H45)</f>
+        <f>(C45*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D45*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F45*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G45*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H45*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C45:H45)</f>
         <v>9.7530134357005736</v>
       </c>
       <c r="T45" s="58">
@@ -13604,7 +13924,7 @@
         <v>10390.65006635699</v>
       </c>
       <c r="S46" s="39">
-        <f>(C46*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D46*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F46*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G46*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H46*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C46:H46)</f>
+        <f>(C46*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D46*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+F46*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G46*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H46*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C46:H46)</f>
         <v>9.9827522935779811</v>
       </c>
       <c r="T46" s="58">
@@ -13730,7 +14050,7 @@
         <v>10445.650076811111</v>
       </c>
       <c r="S47" s="39">
-        <f>(C47*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D47*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F47*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G47*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H47*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C47:H47)</f>
+        <f>(C47*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D47*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F47*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G47*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H47*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C47:H47)</f>
         <v>10.432495088408643</v>
       </c>
       <c r="T47" s="58">
@@ -13856,7 +14176,7 @@
         <v>10159.070073242085</v>
       </c>
       <c r="S48" s="39">
-        <f>(C48*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D48*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F48*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G48*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H48*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C48:H48)</f>
+        <f>(C48*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D48*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F48*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G48*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H48*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C48:H48)</f>
         <v>10.371764705882352</v>
       </c>
       <c r="T48" s="58">
@@ -13982,7 +14302,7 @@
         <v>9517.1600561698524</v>
       </c>
       <c r="S49" s="39">
-        <f>(C49*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D49*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F49*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G49*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H49*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C49:H49)</f>
+        <f>(C49*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D49*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F49*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G49*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H49*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C49:H49)</f>
         <v>10.248048523206753</v>
       </c>
       <c r="T49" s="58">
@@ -14108,7 +14428,7 @@
         <v>10498.68008928211</v>
       </c>
       <c r="S50" s="39">
-        <f>(C50*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D50*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F50*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G50*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H50*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C50:H50)</f>
+        <f>(C50*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D50*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F50*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G50*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H50*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C50:H50)</f>
         <v>10.709343283582088</v>
       </c>
       <c r="T50" s="58">
@@ -14234,7 +14554,7 @@
         <v>10695.460065766629</v>
       </c>
       <c r="S51" s="39">
-        <f>(C51*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D51*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F51*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G51*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H51*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C51:H51)</f>
+        <f>(C51*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D51*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F51*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G51*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H51*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C51:H51)</f>
         <v>10.183500473036897</v>
       </c>
       <c r="T51" s="58">
@@ -14360,7 +14680,7 @@
         <v>10509.270050507781</v>
       </c>
       <c r="S52" s="39">
-        <f>(C52*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D52*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F52*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G52*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H52*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C52:H52)</f>
+        <f>(C52*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D52*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F52*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G52*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H52*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C52:H52)</f>
         <v>10.298216374269007</v>
       </c>
       <c r="T52" s="58">
@@ -14486,7 +14806,7 @@
         <v>8957.2600385557525</v>
       </c>
       <c r="S53" s="39">
-        <f>(C53*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D53*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F53*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G53*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H53*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C53:H53)</f>
+        <f>(C53*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D53*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F53*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G53*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H53*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C53:H53)</f>
         <v>10.46601931330472</v>
       </c>
       <c r="T53" s="58">
@@ -14612,7 +14932,7 @@
         <v>10680.940074127277</v>
       </c>
       <c r="S54" s="39">
-        <f>(C54*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D54*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F54*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G54*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H54*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C54:H54)</f>
+        <f>(C54*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D54*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F54*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G54*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H54*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C54:H54)</f>
         <v>10.615456273764257</v>
       </c>
       <c r="T54" s="58">
@@ -14738,7 +15058,7 @@
         <v>11479.630099581571</v>
       </c>
       <c r="S55" s="39">
-        <f>(C55*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D55*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F55*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G55*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H55*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C55:H55)</f>
+        <f>(C55*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D55*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F55*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G55*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H55*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C55:H55)</f>
         <v>10.290008857395923</v>
       </c>
       <c r="T55" s="58">
@@ -14864,7 +15184,7 @@
         <v>10388.250070320999</v>
       </c>
       <c r="S56" s="39">
-        <f>(C56*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D56*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F56*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G56*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H56*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C56:H56)</f>
+        <f>(C56*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D56*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F56*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G56*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H56*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C56:H56)</f>
         <v>10.352050092764379</v>
       </c>
       <c r="T56" s="62">
@@ -14990,7 +15310,7 @@
         <v>13546.730072406823</v>
       </c>
       <c r="S57" s="39">
-        <f>(C57*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D57*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F57*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G57*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H57*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C57:H57)</f>
+        <f>(C57*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D57*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F57*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G57*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H57*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C57:H57)</f>
         <v>10.372683851402577</v>
       </c>
       <c r="T57" s="62">
@@ -15116,7 +15436,7 @@
         <v>12315.579451853017</v>
       </c>
       <c r="S58" s="39">
-        <f>(C58*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D58*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F58*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G58*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H58*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C58:H58)</f>
+        <f>(C58*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D58*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F58*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G58*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H58*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C58:H58)</f>
         <v>9.8922546634225466</v>
       </c>
       <c r="T58" s="62">
@@ -15242,7 +15562,7 @@
         <v>10160.260072379077</v>
       </c>
       <c r="S59" s="39">
-        <f>(C59*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D59*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F59*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G59*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H59*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C59:H59)</f>
+        <f>(C59*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D59*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F59*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G59*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H59*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C59:H59)</f>
         <v>10.178948412698414</v>
       </c>
       <c r="T59" s="62">
@@ -15368,7 +15688,7 @@
         <v>11897.101568576896</v>
       </c>
       <c r="S60" s="39">
-        <f>(C60*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D60*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F60*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G60*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H60*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C60:H60)</f>
+        <f>(C60*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D60*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F60*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G60*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H60*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C60:H60)</f>
         <v>10.163086319218241</v>
       </c>
       <c r="T60" s="58">
@@ -15494,7 +15814,7 @@
         <v>11115.248564756723</v>
       </c>
       <c r="S61" s="39">
-        <f>(C61*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D61*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F61*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G61*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H61*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C61:H61)</f>
+        <f>(C61*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D61*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F61*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G61*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H61*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C61:H61)</f>
         <v>10.126496872207328</v>
       </c>
       <c r="T61" s="58">
@@ -15620,7 +15940,7 @@
         <v>9521.3653049488476</v>
       </c>
       <c r="S62" s="39">
-        <f>(C62*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D62*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F62*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G62*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H62*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C62:H62)</f>
+        <f>(C62*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D62*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F62*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G62*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H62*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C62:H62)</f>
         <v>9.8342971086739794</v>
       </c>
       <c r="T62" s="58">
@@ -15746,7 +16066,7 @@
         <v>8389.7318373934941</v>
       </c>
       <c r="S63" s="39">
-        <f>(C63*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D63*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F63*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G63*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H63*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C63:H63)</f>
+        <f>(C63*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D63*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+F63*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G63*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H63*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C63:H63)</f>
         <v>10.037154195011338</v>
       </c>
       <c r="T63" s="58">
@@ -15872,7 +16192,7 @@
         <v>9194.5015460136165</v>
       </c>
       <c r="S64" s="39">
-        <f>(C64*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D64*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F64*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G64*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H64*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C64:H64)</f>
+        <f>(C64*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D64*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F64*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G64*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H64*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C64:H64)</f>
         <v>11.535195140278923</v>
       </c>
       <c r="T64" s="58">
@@ -15998,7 +16318,7 @@
         <v>9137.8953052371253</v>
       </c>
       <c r="S65" s="39">
-        <f>(C65*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D65*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F65*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G65*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H65*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C65:H65)</f>
+        <f>(C65*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D65*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F65*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G65*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H65*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C65:H65)</f>
         <v>11.479287543213465</v>
       </c>
       <c r="T65" s="58">
@@ -16124,7 +16444,7 @@
         <v>8583.4766197617519</v>
       </c>
       <c r="S66" s="39">
-        <f>(C66*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D66*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F66*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G66*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H66*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C66:H66)</f>
+        <f>(C66*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D66*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F66*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G66*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H66*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C66:H66)</f>
         <v>11.595632666089708</v>
       </c>
       <c r="T66" s="58">
@@ -16250,7 +16570,7 @@
         <v>8528.8979226116535</v>
       </c>
       <c r="S67" s="39">
-        <f>(C67*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D67*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F67*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G67*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H67*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C67:H67)</f>
+        <f>(C67*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D67*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F67*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G67*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H67*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C67:H67)</f>
         <v>11.464338752116907</v>
       </c>
       <c r="T67" s="58">
@@ -16373,7 +16693,7 @@
         <v>10477.49760604591</v>
       </c>
       <c r="S68" s="39">
-        <f>(C68*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D68*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F68*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G68*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H68*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C68:H68)</f>
+        <f>(C68*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D68*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F68*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G68*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H68*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C68:H68)</f>
         <v>11.126582943518182</v>
       </c>
       <c r="T68" s="62">
@@ -16496,7 +16816,7 @@
         <v>10061.436848239848</v>
       </c>
       <c r="S69" s="39">
-        <f>(C69*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D69*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F69*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G69*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H69*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C69:H69)</f>
+        <f>(C69*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D69*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F69*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G69*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H69*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C69:H69)</f>
         <v>11.310968636358051</v>
       </c>
       <c r="T69" s="62">
@@ -16619,7 +16939,7 @@
         <v>9787.2643356568587</v>
       </c>
       <c r="S70" s="39">
-        <f>(C70*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D70*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F70*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G70*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H70*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C70:H70)</f>
+        <f>(C70*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D70*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F70*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G70*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H70*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C70:H70)</f>
         <v>11.221234641346275</v>
       </c>
       <c r="T70" s="62">
@@ -16742,7 +17062,7 @@
         <v>9172.3808871874426</v>
       </c>
       <c r="S71" s="39">
-        <f>(C71*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D71*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F71*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G71*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H71*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C71:H71)</f>
+        <f>(C71*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D71*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F71*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G71*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H71*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C71:H71)</f>
         <v>11.285605659983291</v>
       </c>
       <c r="T71" s="62">
@@ -16865,7 +17185,7 @@
         <v>9865.6275753044793</v>
       </c>
       <c r="S72" s="39">
-        <f>(C72*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D72*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F72*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G72*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H72*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C72:H72)</f>
+        <f>(C72*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D72*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F72*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G72*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H72*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C72:H72)</f>
         <v>11.114407898658484</v>
       </c>
       <c r="T72" s="58">
@@ -16988,7 +17308,7 @@
         <v>9865.6275753044793</v>
       </c>
       <c r="S73" s="39">
-        <f>(C73*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C73:H73)</f>
+        <f>(C73*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C73:H73)</f>
         <v>11.114407898658484</v>
       </c>
       <c r="T73" s="58">
@@ -17111,7 +17431,7 @@
         <v>10035.797564554641</v>
       </c>
       <c r="S74" s="39">
-        <f>(C74*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C74:H74)</f>
+        <f>(C74*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C74:H74)</f>
         <v>11.04192748686437</v>
       </c>
       <c r="T74" s="58">
@@ -17234,7 +17554,7 @@
         <v>9735.5620722675285</v>
       </c>
       <c r="S75" s="39">
-        <f>(C75*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C75:H75)</f>
+        <f>(C75*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C75:H75)</f>
         <v>11.255394322236393</v>
       </c>
       <c r="T75" s="58">
@@ -17357,7 +17677,7 @@
         <v>8499.6631640485248</v>
       </c>
       <c r="S76" s="39">
-        <f>(C76*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C76:H76)</f>
+        <f>(C76*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C76:H76)</f>
         <v>11.423440717089179</v>
       </c>
       <c r="T76" s="58">
@@ -17480,7 +17800,7 @@
         <v>8787.071993034162</v>
       </c>
       <c r="S77" s="39">
-        <f>(C77*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C77:H77)</f>
+        <f>(C77*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C77:H77)</f>
         <v>11.293444063808437</v>
       </c>
       <c r="T77" s="58">
@@ -17574,7 +17894,7 @@
         <v>5</v>
       </c>
       <c r="J78" s="50">
-        <f>SUM(C78:I78)</f>
+        <f t="shared" ref="J78:J86" si="157">SUM(C78:I78)</f>
         <v>1002</v>
       </c>
       <c r="K78" s="38">
@@ -17599,72 +17919,72 @@
         <v>290.68</v>
       </c>
       <c r="R78" s="38">
-        <f>SUM(K78:Q78)</f>
+        <f t="shared" ref="R78:R89" si="158">SUM(K78:Q78)</f>
         <v>12167.569999999998</v>
       </c>
       <c r="S78" s="39">
-        <f>(C78*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D78*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F78*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G78*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H78*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C78:H78)</f>
+        <f>(C78*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D78*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F78*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G78*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H78*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C78:H78)</f>
         <v>11.684642267445613</v>
       </c>
       <c r="T78" s="58">
-        <f>$K78/SUM($K78:$Q78)</f>
+        <f t="shared" ref="T78:T86" si="159">$K78/SUM($K78:$Q78)</f>
         <v>3.4978224904397531E-2</v>
       </c>
       <c r="U78" s="58">
-        <f>L78/SUM($K78:$Q78)</f>
+        <f t="shared" ref="U78:U86" si="160">L78/SUM($K78:$Q78)</f>
         <v>0.60128604150212384</v>
       </c>
       <c r="V78" s="58">
-        <f t="shared" ref="V78:Y80" si="157">M78/SUM($K$2:$Q$2)</f>
+        <f t="shared" ref="V78:Y80" si="161">M78/SUM($K$2:$Q$2)</f>
         <v>0.51064847368555877</v>
       </c>
       <c r="W78" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.38283547460507711</v>
       </c>
       <c r="X78" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.16972366064947003</v>
       </c>
       <c r="Y78" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.11397468051732138</v>
       </c>
       <c r="Z78" s="58"/>
       <c r="AA78" s="58">
-        <f>R78/SUM($K78:$Q78)</f>
+        <f t="shared" ref="AA78:AA86" si="162">R78/SUM($K78:$Q78)</f>
         <v>1</v>
       </c>
       <c r="AB78" s="58">
-        <f t="shared" ref="AB78:AH80" si="158">K78/SUM($K78:$P78)</f>
+        <f t="shared" ref="AB78:AH80" si="163">K78/SUM($K78:$P78)</f>
         <v>3.583429668877966E-2</v>
       </c>
       <c r="AC78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.61600216891795723</v>
       </c>
       <c r="AD78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.15102943615710845</v>
       </c>
       <c r="AE78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.11322745264122182</v>
       </c>
       <c r="AF78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>5.0197484358278983E-2</v>
       </c>
       <c r="AG78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>3.3709161236653712E-2</v>
       </c>
       <c r="AH78" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>2.447442049223324E-2</v>
       </c>
       <c r="AI78" s="59">
-        <f>SUM($AB78:$AH78)</f>
+        <f t="shared" ref="AI78:AI86" si="164">SUM($AB78:$AH78)</f>
         <v>1.0244744204922329</v>
       </c>
     </row>
@@ -17697,7 +18017,7 @@
         <v>9</v>
       </c>
       <c r="J79" s="50">
-        <f>SUM(C79:I79)</f>
+        <f t="shared" si="157"/>
         <v>1038</v>
       </c>
       <c r="K79" s="38">
@@ -17722,72 +18042,72 @@
         <v>493.77</v>
       </c>
       <c r="R79" s="38">
-        <f>SUM(K79:Q79)</f>
+        <f t="shared" si="158"/>
         <v>12361.339999999997</v>
       </c>
       <c r="S79" s="39">
-        <f>(C79*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D79*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F79*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G79*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H79*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C79:H79)</f>
+        <f>(C79*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D79*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F79*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G79*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H79*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C79:H79)</f>
         <v>11.446303293665002</v>
       </c>
       <c r="T79" s="58">
-        <f>$K79/SUM($K79:$Q79)</f>
+        <f t="shared" si="159"/>
         <v>2.6520587573839093E-2</v>
       </c>
       <c r="U79" s="58">
-        <f>L79/SUM($K79:$Q79)</f>
+        <f t="shared" si="160"/>
         <v>0.62639649099531269</v>
       </c>
       <c r="V79" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.46041944823227621</v>
       </c>
       <c r="W79" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.36778441715940147</v>
       </c>
       <c r="X79" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.1156656826211102</v>
       </c>
       <c r="Y79" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.13695978318733959</v>
       </c>
       <c r="Z79" s="58"/>
       <c r="AA79" s="58">
-        <f>R79/SUM($K79:$Q79)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>2.7624020755723382E-2</v>
       </c>
       <c r="AC79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.65245875945960274</v>
       </c>
       <c r="AD79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.13628063706386395</v>
       </c>
       <c r="AE79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.1088613760019955</v>
       </c>
       <c r="AF79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>3.4236157865510819E-2</v>
       </c>
       <c r="AG79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>4.0539048853303575E-2</v>
       </c>
       <c r="AH79" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>4.1606664211797373E-2</v>
       </c>
       <c r="AI79" s="59">
-        <f>SUM($AB79:$AH79)</f>
+        <f t="shared" si="164"/>
         <v>1.0416066642117974</v>
       </c>
     </row>
@@ -17820,7 +18140,7 @@
         <v>9</v>
       </c>
       <c r="J80" s="50">
-        <f>SUM(C80:I80)</f>
+        <f t="shared" si="157"/>
         <v>913</v>
       </c>
       <c r="K80" s="38">
@@ -17845,72 +18165,72 @@
         <v>739</v>
       </c>
       <c r="R80" s="38">
-        <f>SUM(K80:Q80)</f>
+        <f t="shared" si="158"/>
         <v>10766.76</v>
       </c>
       <c r="S80" s="39">
-        <f>(C80*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D80*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+F80*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G80*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H80*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C80:H80)</f>
+        <f>(C80*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D80*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+F80*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G80*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H80*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C80:H80)</f>
         <v>10.719660851866944</v>
       </c>
       <c r="T80" s="58">
-        <f>$K80/SUM($K80:$Q80)</f>
+        <f t="shared" si="159"/>
         <v>2.3767595822698752E-2</v>
       </c>
       <c r="U80" s="58">
-        <f>L80/SUM($K80:$Q80)</f>
+        <f t="shared" si="160"/>
         <v>0.59794125623678807</v>
       </c>
       <c r="V80" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.43720090756139829</v>
       </c>
       <c r="W80" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.2736462731053802</v>
       </c>
       <c r="X80" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>8.3064073037626196E-2</v>
       </c>
       <c r="Y80" s="58">
-        <f t="shared" si="157"/>
+        <f t="shared" si="161"/>
         <v>0.15520495571794993</v>
       </c>
       <c r="Z80" s="58"/>
       <c r="AA80" s="58">
-        <f>R80/SUM($K80:$Q80)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>2.5519158815129204E-2</v>
       </c>
       <c r="AC80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.64200678915331044</v>
       </c>
       <c r="AD80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>0.15315085323142949</v>
       </c>
       <c r="AE80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>9.5857898473836647E-2</v>
       </c>
       <c r="AF80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>2.9097226100345437E-2</v>
       </c>
       <c r="AG80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>5.4368074225948762E-2</v>
       </c>
       <c r="AH80" s="58">
-        <f t="shared" si="158"/>
+        <f t="shared" si="163"/>
         <v>7.3695421509888545E-2</v>
       </c>
       <c r="AI80" s="59">
-        <f>SUM($AB80:$AH80)</f>
+        <f t="shared" si="164"/>
         <v>1.0736954215098886</v>
       </c>
     </row>
@@ -17943,7 +18263,7 @@
         <v>2</v>
       </c>
       <c r="J81" s="50">
-        <f>SUM(C81:I81)</f>
+        <f t="shared" si="157"/>
         <v>741</v>
       </c>
       <c r="K81" s="38">
@@ -17968,72 +18288,72 @@
         <v>211.8</v>
       </c>
       <c r="R81" s="38">
-        <f>SUM(K81:Q81)</f>
+        <f t="shared" si="158"/>
         <v>8658.64</v>
       </c>
       <c r="S81" s="39">
-        <f>(C81*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D81*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F81*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G81*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H81*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C81:H81)</f>
+        <f>(C81*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D81*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F81*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G81*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H81*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C81:H81)</f>
         <v>10.90544471943277</v>
       </c>
       <c r="T81" s="41">
-        <f>$K81/SUM($K81:$Q81)</f>
+        <f t="shared" si="159"/>
         <v>4.9175159147394981E-2</v>
       </c>
       <c r="U81" s="41">
-        <f>L81/SUM($K81:$Q81)</f>
+        <f t="shared" si="160"/>
         <v>0.61338270213336055</v>
       </c>
       <c r="V81" s="41">
-        <f>M81/SUM($K$2:$Q$2)</f>
+        <f t="shared" ref="V81:Y86" si="165">M81/SUM($K$2:$Q$2)</f>
         <v>0.36783281284250607</v>
       </c>
       <c r="W81" s="41">
-        <f>N81/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.20223132567163232</v>
       </c>
       <c r="X81" s="41">
-        <f>O81/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>9.4943789837475839E-2</v>
       </c>
       <c r="Y81" s="41">
-        <f>P81/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.10647334963603602</v>
       </c>
       <c r="Z81" s="41"/>
       <c r="AA81" s="41">
-        <f>R81/SUM($K81:$Q81)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB81" s="41">
-        <f>K81/SUM($K81:$P81)</f>
+        <f t="shared" ref="AB81:AH86" si="166">K81/SUM($K81:$P81)</f>
         <v>5.040819998958191E-2</v>
       </c>
       <c r="AC81" s="41">
-        <f>L81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>0.62876294566962321</v>
       </c>
       <c r="AD81" s="41">
-        <f>M81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>0.15296726349735518</v>
       </c>
       <c r="AE81" s="41">
-        <f>N81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>8.4100089500925748E-2</v>
       </c>
       <c r="AF81" s="41">
-        <f>O81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>3.9483404444739079E-2</v>
       </c>
       <c r="AG81" s="41">
-        <f>P81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>4.4278096897774809E-2</v>
       </c>
       <c r="AH81" s="41">
-        <f>Q81/SUM($K81:$P81)</f>
+        <f t="shared" si="166"/>
         <v>2.5074465717357025E-2</v>
       </c>
       <c r="AI81" s="51">
-        <f>SUM($AB81:$AH81)</f>
+        <f t="shared" si="164"/>
         <v>1.0250744657173569</v>
       </c>
     </row>
@@ -18066,7 +18386,7 @@
         <v>6</v>
       </c>
       <c r="J82" s="50">
-        <f>SUM(C82:I82)</f>
+        <f t="shared" si="157"/>
         <v>888</v>
       </c>
       <c r="K82" s="38">
@@ -18091,72 +18411,72 @@
         <v>322</v>
       </c>
       <c r="R82" s="38">
-        <f>SUM(K82:Q82)</f>
+        <f t="shared" si="158"/>
         <v>10416.629999999997</v>
       </c>
       <c r="S82" s="39">
-        <f>(C82*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D82*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F82*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G82*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H82*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C82:H82)</f>
+        <f>(C82*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D82*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F82*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G82*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H82*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C82:H82)</f>
         <v>11.223761205261834</v>
       </c>
       <c r="T82" s="41">
-        <f>$K82/SUM($K82:$Q82)</f>
+        <f t="shared" si="159"/>
         <v>4.1684306728759717E-2</v>
       </c>
       <c r="U82" s="41">
-        <f>L82/SUM($K82:$Q82)</f>
+        <f t="shared" si="160"/>
         <v>0.57828683556966121</v>
       </c>
       <c r="V82" s="41">
-        <f>M82/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.46595648374047366</v>
       </c>
       <c r="W82" s="41">
-        <f>N82/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.26326682248178745</v>
       </c>
       <c r="X82" s="41">
-        <f>O82/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.18217843203680345</v>
       </c>
       <c r="Y82" s="41">
-        <f>P82/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.12387302111475181</v>
       </c>
       <c r="Z82" s="41"/>
       <c r="AA82" s="41">
-        <f>R82/SUM($K82:$Q82)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB82" s="41">
-        <f>K82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>4.3013958906864373E-2</v>
       </c>
       <c r="AC82" s="41">
-        <f>L82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>0.59673311453713507</v>
       </c>
       <c r="AD82" s="41">
-        <f>M82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>0.16214264415832971</v>
       </c>
       <c r="AE82" s="41">
-        <f>N82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>9.1611084309182203E-2</v>
       </c>
       <c r="AF82" s="41">
-        <f>O82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>6.3394101616403978E-2</v>
       </c>
       <c r="AG82" s="41">
-        <f>P82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>4.3105096472084665E-2</v>
       </c>
       <c r="AH82" s="41">
-        <f>Q82/SUM($K82:$P82)</f>
+        <f t="shared" si="166"/>
         <v>3.1898147827112047E-2</v>
       </c>
       <c r="AI82" s="51">
-        <f>SUM($AB82:$AH82)</f>
+        <f t="shared" si="164"/>
         <v>1.0318981478271121</v>
       </c>
     </row>
@@ -18189,7 +18509,7 @@
         <v>3</v>
       </c>
       <c r="J83" s="50">
-        <f>SUM(C83:I83)</f>
+        <f t="shared" si="157"/>
         <v>919</v>
       </c>
       <c r="K83" s="38">
@@ -18214,72 +18534,72 @@
         <v>178</v>
       </c>
       <c r="R83" s="38">
-        <f>SUM(K83:Q83)</f>
+        <f t="shared" si="158"/>
         <v>10609.250000000007</v>
       </c>
       <c r="S83" s="39">
-        <f>(C83*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D83*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F83*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G83*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H83*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C83:H83)</f>
+        <f>(C83*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D83*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F83*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G83*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H83*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C83:H83)</f>
         <v>11.233651387612044</v>
       </c>
       <c r="T83" s="41">
-        <f>$K83/SUM($K83:$Q83)</f>
+        <f t="shared" si="159"/>
         <v>3.8651177038904708E-2</v>
       </c>
       <c r="U83" s="41">
-        <f>L83/SUM($K83:$Q83)</f>
+        <f t="shared" si="160"/>
         <v>0.62477083676979994</v>
       </c>
       <c r="V83" s="41">
-        <f>M83/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.40051982657264618</v>
       </c>
       <c r="W83" s="41">
-        <f>N83/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.33454512328088587</v>
       </c>
       <c r="X83" s="41">
-        <f>O83/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>9.2669192731537745E-2</v>
       </c>
       <c r="Y83" s="41">
-        <f>P83/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.13814120721608109</v>
       </c>
       <c r="Z83" s="41"/>
       <c r="AA83" s="41">
-        <f>R83/SUM($K83:$Q83)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB83" s="41">
-        <f>K83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>3.9310724985020952E-2</v>
       </c>
       <c r="AC83" s="41">
-        <f>L83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>0.63543199520671068</v>
       </c>
       <c r="AD83" s="41">
-        <f>M83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>0.13487453565008978</v>
       </c>
       <c r="AE83" s="41">
-        <f>N83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>0.11265763930497304</v>
       </c>
       <c r="AF83" s="41">
-        <f>O83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>3.1206231276213279E-2</v>
       </c>
       <c r="AG83" s="41">
-        <f>P83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>4.6518873576992199E-2</v>
       </c>
       <c r="AH83" s="41">
-        <f>Q83/SUM($K83:$P83)</f>
+        <f t="shared" si="166"/>
         <v>1.7064110245656069E-2</v>
       </c>
       <c r="AI83" s="51">
-        <f>SUM($AB83:$AH83)</f>
+        <f t="shared" si="164"/>
         <v>1.0170641102456561</v>
       </c>
     </row>
@@ -18312,7 +18632,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="50">
-        <f>SUM(C84:I84)</f>
+        <f t="shared" si="157"/>
         <v>849</v>
       </c>
       <c r="K84" s="38">
@@ -18337,72 +18657,72 @@
         <v>56</v>
       </c>
       <c r="R84" s="38">
-        <f>SUM(K84:Q84)</f>
+        <f t="shared" si="158"/>
         <v>9822.1100000000042</v>
       </c>
       <c r="S84" s="39">
-        <f>(C84*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D84*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F84*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G84*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H84*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C84:H84)</f>
+        <f>(C84*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D84*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F84*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G84*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H84*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C84:H84)</f>
         <v>11.770956898962281</v>
       </c>
       <c r="T84" s="41">
-        <f>$K84/SUM($K84:$Q84)</f>
+        <f t="shared" si="159"/>
         <v>5.4594175793184943E-2</v>
       </c>
       <c r="U84" s="41">
-        <f>L84/SUM($K84:$Q84)</f>
+        <f t="shared" si="160"/>
         <v>0.56914145738542943</v>
       </c>
       <c r="V84" s="41">
-        <f>M84/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.33492944194083774</v>
       </c>
       <c r="W84" s="41">
-        <f>N84/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.3170002647528547</v>
       </c>
       <c r="X84" s="41">
-        <f>O84/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.27110692314480833</v>
       </c>
       <c r="Y84" s="41">
-        <f>P84/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.1131177922458728</v>
       </c>
       <c r="Z84" s="41"/>
       <c r="AA84" s="41">
-        <f>R84/SUM($K84:$Q84)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB84" s="41">
-        <f>K84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>5.490722508757323E-2</v>
       </c>
       <c r="AC84" s="41">
-        <f>L84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>0.57240498007906937</v>
       </c>
       <c r="AD84" s="41">
-        <f>M84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>0.12046864104541109</v>
       </c>
       <c r="AE84" s="41">
-        <f>N84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>0.11401980932018992</v>
       </c>
       <c r="AF84" s="41">
-        <f>O84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>9.7512725128019187E-2</v>
       </c>
       <c r="AG84" s="41">
-        <f>P84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>4.0686619339737086E-2</v>
       </c>
       <c r="AH84" s="41">
-        <f>Q84/SUM($K84:$P84)</f>
+        <f t="shared" si="166"/>
         <v>5.7341152209016664E-3</v>
       </c>
       <c r="AI84" s="51">
-        <f>SUM($AB84:$AH84)</f>
+        <f t="shared" si="164"/>
         <v>1.0057341152209016</v>
       </c>
     </row>
@@ -18414,119 +18734,119 @@
         <v>5</v>
       </c>
       <c r="C85" s="50">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D85" s="50">
-        <v>426</v>
+        <v>272</v>
       </c>
       <c r="E85" s="50">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="F85" s="50">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G85" s="50">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H85" s="45">
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="I85" s="50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J85" s="50">
-        <f>SUM(C85:I85)</f>
-        <v>859</v>
+        <f t="shared" si="157"/>
+        <v>543</v>
       </c>
       <c r="K85" s="38">
-        <v>318.98</v>
+        <v>186.70999999999998</v>
       </c>
       <c r="L85" s="38">
-        <v>6116.5200000000013</v>
+        <v>3888.4700000000025</v>
       </c>
       <c r="M85" s="38">
-        <v>1506.5</v>
+        <v>888.08000000000015</v>
       </c>
       <c r="N85" s="38">
-        <v>1000.8699999999995</v>
+        <v>506.73999999999961</v>
       </c>
       <c r="O85" s="38">
-        <v>644.90999999999985</v>
+        <v>523.82000000000005</v>
       </c>
       <c r="P85" s="38">
-        <v>422.70999999999992</v>
+        <v>255.66000000000025</v>
       </c>
       <c r="Q85" s="38">
-        <v>223</v>
+        <v>83</v>
       </c>
       <c r="R85" s="38">
-        <f>SUM(K85:Q85)</f>
-        <v>10233.49</v>
+        <f t="shared" si="158"/>
+        <v>6332.4800000000023</v>
       </c>
       <c r="S85" s="39">
-        <f>(C85*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D85*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F85*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G85*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H85*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C85:H85)</f>
-        <v>11.432785386956674</v>
+        <f>(C85*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D85*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F85*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G85*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H85*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C85:H85)</f>
+        <v>11.475167547642982</v>
       </c>
       <c r="T85" s="41">
-        <f>$K85/SUM($K85:$Q85)</f>
-        <v>3.1170206840481596E-2</v>
+        <f t="shared" si="159"/>
+        <v>2.9484498964070936E-2</v>
       </c>
       <c r="U85" s="41">
-        <f>L85/SUM($K85:$Q85)</f>
-        <v>0.59769638705856964</v>
+        <f t="shared" si="160"/>
+        <v>0.61405168275304478</v>
       </c>
       <c r="V85" s="41">
-        <f>M85/SUM($K$2:$Q$2)</f>
-        <v>0.42887115645754981</v>
+        <f t="shared" si="165"/>
+        <v>0.25281904854087017</v>
       </c>
       <c r="W85" s="41">
-        <f>N85/SUM($K$2:$Q$2)</f>
-        <v>0.2849281608786377</v>
+        <f t="shared" si="165"/>
+        <v>0.14425899092153907</v>
       </c>
       <c r="X85" s="41">
-        <f>O85/SUM($K$2:$Q$2)</f>
-        <v>0.18359329406640451</v>
+        <f t="shared" si="165"/>
+        <v>0.14912133367115418</v>
       </c>
       <c r="Y85" s="41">
-        <f>P85/SUM($K$2:$Q$2)</f>
-        <v>0.1203372894431934</v>
+        <f t="shared" si="165"/>
+        <v>7.2781413780243803E-2</v>
       </c>
       <c r="Z85" s="41"/>
       <c r="AA85" s="41">
-        <f>R85/SUM($K85:$Q85)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB85" s="41">
-        <f>K85/SUM($K85:$P85)</f>
-        <v>3.1864574061809162E-2</v>
+        <f t="shared" si="166"/>
+        <v>2.9876085690329422E-2</v>
       </c>
       <c r="AC85" s="41">
-        <f>L85/SUM($K85:$P85)</f>
-        <v>0.61101104940916995</v>
+        <f t="shared" si="166"/>
+        <v>0.62220696761970617</v>
       </c>
       <c r="AD85" s="41">
-        <f>M85/SUM($K85:$P85)</f>
-        <v>0.15049213375169448</v>
+        <f t="shared" si="166"/>
+        <v>0.14210462310464228</v>
       </c>
       <c r="AE85" s="41">
-        <f>N85/SUM($K85:$P85)</f>
-        <v>9.9982118757423424E-2</v>
+        <f t="shared" si="166"/>
+        <v>8.1085146284170753E-2</v>
       </c>
       <c r="AF85" s="41">
-        <f>O85/SUM($K85:$P85)</f>
-        <v>6.4423419832595599E-2</v>
+        <f t="shared" si="166"/>
+        <v>8.3818173672049495E-2</v>
       </c>
       <c r="AG85" s="41">
-        <f>P85/SUM($K85:$P85)</f>
-        <v>4.2226704187307507E-2</v>
+        <f t="shared" si="166"/>
+        <v>4.0909003629101964E-2</v>
       </c>
       <c r="AH85" s="41">
-        <f>Q85/SUM($K85:$P85)</f>
-        <v>2.2276631813227924E-2</v>
+        <f t="shared" si="166"/>
+        <v>1.3281104987934991E-2</v>
       </c>
       <c r="AI85" s="51">
-        <f>SUM($AB85:$AH85)</f>
-        <v>1.0222766318132281</v>
+        <f t="shared" si="164"/>
+        <v>1.0132811049879349</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
@@ -18558,7 +18878,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="50">
-        <f>SUM(C86:I86)</f>
+        <f t="shared" si="157"/>
         <v>731</v>
       </c>
       <c r="K86" s="38">
@@ -18583,73 +18903,442 @@
         <v>142</v>
       </c>
       <c r="R86" s="38">
-        <f>SUM(K86:Q86)</f>
+        <f t="shared" si="158"/>
         <v>8333.9299999999967</v>
       </c>
       <c r="S86" s="39">
-        <f>(C86*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D86*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F86*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G86*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H86*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C86:H86)</f>
+        <f>(C86*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D86*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F86*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G86*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H86*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C86:H86)</f>
         <v>12.08826491167906</v>
       </c>
       <c r="T86" s="41">
-        <f>$K86/SUM($K86:$Q86)</f>
+        <f t="shared" si="159"/>
         <v>5.2496241269125166E-2</v>
       </c>
       <c r="U86" s="41">
-        <f>L86/SUM($K86:$Q86)</f>
+        <f t="shared" si="160"/>
         <v>0.63096762271821327</v>
       </c>
       <c r="V86" s="41">
-        <f>M86/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.22856142408567745</v>
       </c>
       <c r="W86" s="41">
-        <f>N86/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.223835727970712</v>
       </c>
       <c r="X86" s="41">
-        <f>O86/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>0.16761702503195539</v>
       </c>
       <c r="Y86" s="41">
-        <f>P86/SUM($K$2:$Q$2)</f>
+        <f t="shared" si="165"/>
         <v>9.0545476284691881E-2</v>
       </c>
       <c r="Z86" s="41"/>
       <c r="AA86" s="41">
-        <f>R86/SUM($K86:$Q86)</f>
+        <f t="shared" si="162"/>
         <v>1</v>
       </c>
       <c r="AB86" s="41">
-        <f>K86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>5.3406218070711088E-2</v>
       </c>
       <c r="AC86" s="41">
-        <f>L86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>0.64190489908971382</v>
       </c>
       <c r="AD86" s="41">
-        <f>M86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>9.8007429262701271E-2</v>
       </c>
       <c r="AE86" s="41">
-        <f>N86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>9.5981044759903975E-2</v>
       </c>
       <c r="AF86" s="41">
-        <f>O86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>7.1874393457951949E-2</v>
       </c>
       <c r="AG86" s="41">
-        <f>P86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>3.882601535901798E-2</v>
       </c>
       <c r="AH86" s="41">
-        <f>Q86/SUM($K86:$P86)</f>
+        <f t="shared" si="166"/>
         <v>1.7334132493807938E-2</v>
       </c>
       <c r="AI86" s="51">
-        <f>SUM($AB86:$AH86)</f>
+        <f t="shared" si="164"/>
         <v>1.0173341324938081</v>
+      </c>
+    </row>
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A87" s="49">
+        <v>2024</v>
+      </c>
+      <c r="B87" s="27">
+        <v>7</v>
+      </c>
+      <c r="C87" s="13">
+        <v>48</v>
+      </c>
+      <c r="D87" s="13">
+        <v>411</v>
+      </c>
+      <c r="E87" s="13">
+        <v>72</v>
+      </c>
+      <c r="F87" s="13">
+        <v>89</v>
+      </c>
+      <c r="G87" s="13">
+        <v>45</v>
+      </c>
+      <c r="H87" s="13">
+        <v>206</v>
+      </c>
+      <c r="I87" s="13">
+        <v>0</v>
+      </c>
+      <c r="J87" s="22">
+        <f t="shared" ref="J87:J89" si="167">SUM(C87:I87)</f>
+        <v>871</v>
+      </c>
+      <c r="K87" s="16">
+        <v>499.1600000000002</v>
+      </c>
+      <c r="L87" s="16">
+        <v>6040.1</v>
+      </c>
+      <c r="M87" s="16">
+        <v>1609.3999999999994</v>
+      </c>
+      <c r="N87" s="16">
+        <v>922.1600000000002</v>
+      </c>
+      <c r="O87" s="16">
+        <v>657.54</v>
+      </c>
+      <c r="P87" s="16">
+        <v>576.5099999999992</v>
+      </c>
+      <c r="Q87" s="16">
+        <v>0</v>
+      </c>
+      <c r="R87" s="38">
+        <f t="shared" si="158"/>
+        <v>10304.869999999999</v>
+      </c>
+      <c r="S87" s="39">
+        <f>(C87*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D87*VLOOKUP($D$1,OP!$A$25:$B$30,2,FALSE)+F87*VLOOKUP($F$1,OP!$A$25:$B$30,2,FALSE)+G87*VLOOKUP($G$1,OP!$A$25:$B$30,2,FALSE)+H87*VLOOKUP($H$1,OP!$A$25:$B$30,2,FALSE))/SUM(C87:H87)</f>
+        <v>10.630912785935369</v>
+      </c>
+      <c r="T87" s="62">
+        <f t="shared" ref="T87:T89" si="168">$K87/SUM($K87:$Q87)</f>
+        <v>4.8439233100466113E-2</v>
+      </c>
+      <c r="U87" s="62">
+        <f t="shared" ref="U87:U89" si="169">L87/SUM($K87:$Q87)</f>
+        <v>0.5861403394705611</v>
+      </c>
+      <c r="V87" s="62">
+        <f t="shared" ref="V87:V89" si="170">M87/SUM($K$2:$Q$2)</f>
+        <v>0.45816477876055783</v>
+      </c>
+      <c r="W87" s="62">
+        <f t="shared" ref="W87:W89" si="171">N87/SUM($K$2:$Q$2)</f>
+        <v>0.26252095960099187</v>
+      </c>
+      <c r="X87" s="62">
+        <f t="shared" ref="X87:X89" si="172">O87/SUM($K$2:$Q$2)</f>
+        <v>0.18718880864062215</v>
+      </c>
+      <c r="Y87" s="62">
+        <f t="shared" ref="Y87:Y89" si="173">P87/SUM($K$2:$Q$2)</f>
+        <v>0.16412114862883617</v>
+      </c>
+      <c r="Z87" s="62"/>
+      <c r="AA87" s="62">
+        <f t="shared" ref="AA87:AA89" si="174">R87/SUM($K87:$Q87)</f>
+        <v>1</v>
+      </c>
+      <c r="AB87" s="62">
+        <f t="shared" ref="AB87:AB89" si="175">K87/SUM($K87:$P87)</f>
+        <v>4.8439233100466113E-2</v>
+      </c>
+      <c r="AC87" s="62">
+        <f t="shared" ref="AC87:AC89" si="176">L87/SUM($K87:$P87)</f>
+        <v>0.5861403394705611</v>
+      </c>
+      <c r="AD87" s="62">
+        <f t="shared" ref="AD87:AD89" si="177">M87/SUM($K87:$P87)</f>
+        <v>0.15617858352410069</v>
+      </c>
+      <c r="AE87" s="62">
+        <f t="shared" ref="AE87:AE89" si="178">N87/SUM($K87:$P87)</f>
+        <v>8.948778587211681E-2</v>
+      </c>
+      <c r="AF87" s="62">
+        <f t="shared" ref="AF87:AF89" si="179">O87/SUM($K87:$P87)</f>
+        <v>6.3808665223336156E-2</v>
+      </c>
+      <c r="AG87" s="62">
+        <f t="shared" ref="AG87:AG89" si="180">P87/SUM($K87:$P87)</f>
+        <v>5.594539280941916E-2</v>
+      </c>
+      <c r="AH87" s="62">
+        <f t="shared" ref="AH87:AH89" si="181">Q87/SUM($K87:$P87)</f>
+        <v>0</v>
+      </c>
+      <c r="AI87" s="63">
+        <f t="shared" ref="AI87:AI89" si="182">SUM($AB87:$AH87)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A88" s="49">
+        <v>2024</v>
+      </c>
+      <c r="B88" s="27">
+        <v>8</v>
+      </c>
+      <c r="C88" s="13">
+        <v>38</v>
+      </c>
+      <c r="D88" s="13">
+        <v>439</v>
+      </c>
+      <c r="E88" s="13">
+        <v>68</v>
+      </c>
+      <c r="F88" s="13">
+        <v>113</v>
+      </c>
+      <c r="G88" s="13">
+        <v>35</v>
+      </c>
+      <c r="H88" s="13">
+        <v>156</v>
+      </c>
+      <c r="I88" s="13">
+        <v>1</v>
+      </c>
+      <c r="J88" s="22">
+        <f t="shared" si="167"/>
+        <v>850</v>
+      </c>
+      <c r="K88" s="16">
+        <v>391.64999999999986</v>
+      </c>
+      <c r="L88" s="16">
+        <v>6531.9899999999907</v>
+      </c>
+      <c r="M88" s="16">
+        <v>1597.7</v>
+      </c>
+      <c r="N88" s="16">
+        <v>994.23999999999967</v>
+      </c>
+      <c r="O88" s="16">
+        <v>507.71</v>
+      </c>
+      <c r="P88" s="16">
+        <v>485.58999999999884</v>
+      </c>
+      <c r="Q88" s="16">
+        <v>67</v>
+      </c>
+      <c r="R88" s="38">
+        <f t="shared" si="158"/>
+        <v>10575.879999999988</v>
+      </c>
+      <c r="S88" s="39">
+        <f>(C88*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D88*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F88*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G88*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H88*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C88:H88)</f>
+        <v>11.733722025912837</v>
+      </c>
+      <c r="T88" s="62">
+        <f t="shared" si="168"/>
+        <v>3.7032379338646081E-2</v>
+      </c>
+      <c r="U88" s="62">
+        <f t="shared" si="169"/>
+        <v>0.61763087327012012</v>
+      </c>
+      <c r="V88" s="62">
+        <f t="shared" si="170"/>
+        <v>0.45483401704097404</v>
+      </c>
+      <c r="W88" s="62">
+        <f t="shared" si="171"/>
+        <v>0.28304072923754009</v>
+      </c>
+      <c r="X88" s="62">
+        <f t="shared" si="172"/>
+        <v>0.14453513099572693</v>
+      </c>
+      <c r="Y88" s="62">
+        <f t="shared" si="173"/>
+        <v>0.13823799858229083</v>
+      </c>
+      <c r="Z88" s="62"/>
+      <c r="AA88" s="62">
+        <f t="shared" si="174"/>
+        <v>1</v>
+      </c>
+      <c r="AB88" s="62">
+        <f t="shared" si="175"/>
+        <v>3.7268481512777792E-2</v>
+      </c>
+      <c r="AC88" s="62">
+        <f t="shared" si="176"/>
+        <v>0.62156861625596616</v>
+      </c>
+      <c r="AD88" s="62">
+        <f t="shared" si="177"/>
+        <v>0.15203332800450683</v>
+      </c>
+      <c r="AE88" s="62">
+        <f t="shared" si="178"/>
+        <v>9.4609511194342383E-2</v>
+      </c>
+      <c r="AF88" s="62">
+        <f t="shared" si="179"/>
+        <v>4.8312474783230995E-2</v>
+      </c>
+      <c r="AG88" s="62">
+        <f t="shared" si="180"/>
+        <v>4.6207588249175875E-2</v>
+      </c>
+      <c r="AH88" s="62">
+        <f t="shared" si="181"/>
+        <v>6.3755604783763895E-3</v>
+      </c>
+      <c r="AI88" s="63">
+        <f t="shared" si="182"/>
+        <v>1.0063755604783764</v>
+      </c>
+    </row>
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A89" s="49">
+        <v>2024</v>
+      </c>
+      <c r="B89" s="49">
+        <v>9</v>
+      </c>
+      <c r="C89" s="13">
+        <v>24</v>
+      </c>
+      <c r="D89" s="13">
+        <v>287</v>
+      </c>
+      <c r="E89" s="13">
+        <v>45</v>
+      </c>
+      <c r="F89" s="13">
+        <v>65</v>
+      </c>
+      <c r="G89" s="13">
+        <v>25</v>
+      </c>
+      <c r="H89" s="13">
+        <v>107</v>
+      </c>
+      <c r="I89" s="13">
+        <v>3</v>
+      </c>
+      <c r="J89" s="50">
+        <f t="shared" si="167"/>
+        <v>556</v>
+      </c>
+      <c r="K89" s="38">
+        <v>292.08999999999997</v>
+      </c>
+      <c r="L89" s="38">
+        <v>4412.5400000000054</v>
+      </c>
+      <c r="M89" s="38">
+        <v>1076.8200000000002</v>
+      </c>
+      <c r="N89" s="38">
+        <v>779.27</v>
+      </c>
+      <c r="O89" s="38">
+        <v>377.31999999999994</v>
+      </c>
+      <c r="P89" s="38">
+        <v>381.18999999999966</v>
+      </c>
+      <c r="Q89" s="38">
+        <v>240</v>
+      </c>
+      <c r="R89" s="38">
+        <f t="shared" si="158"/>
+        <v>7559.2300000000059</v>
+      </c>
+      <c r="S89" s="39">
+        <f>(C89*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D89*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+F89*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G89*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H89*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C89:H89)</f>
+        <v>11.700560578661847</v>
+      </c>
+      <c r="T89" s="58">
+        <f t="shared" si="168"/>
+        <v>3.864017896002632E-2</v>
+      </c>
+      <c r="U89" s="58">
+        <f t="shared" si="169"/>
+        <v>0.58372876602511126</v>
+      </c>
+      <c r="V89" s="58">
+        <f t="shared" si="170"/>
+        <v>0.3065496440070487</v>
+      </c>
+      <c r="W89" s="58">
+        <f t="shared" si="171"/>
+        <v>0.2218429645487387</v>
+      </c>
+      <c r="X89" s="58">
+        <f t="shared" si="172"/>
+        <v>0.1074156420541405</v>
+      </c>
+      <c r="Y89" s="58">
+        <f t="shared" si="173"/>
+        <v>0.10851735554600284</v>
+      </c>
+      <c r="Z89" s="58"/>
+      <c r="AA89" s="58">
+        <f t="shared" si="174"/>
+        <v>1</v>
+      </c>
+      <c r="AB89" s="58">
+        <f t="shared" si="175"/>
+        <v>3.9907203353358171E-2</v>
+      </c>
+      <c r="AC89" s="58">
+        <f t="shared" si="176"/>
+        <v>0.60286942752174777</v>
+      </c>
+      <c r="AD89" s="58">
+        <f t="shared" si="177"/>
+        <v>0.1471220333286424</v>
+      </c>
+      <c r="AE89" s="58">
+        <f t="shared" si="178"/>
+        <v>0.1064688498653546</v>
+      </c>
+      <c r="AF89" s="58">
+        <f t="shared" si="179"/>
+        <v>5.1551870893522901E-2</v>
+      </c>
+      <c r="AG89" s="58">
+        <f t="shared" si="180"/>
+        <v>5.2080615037374059E-2</v>
+      </c>
+      <c r="AH89" s="58">
+        <f t="shared" si="181"/>
+        <v>3.2790334502399814E-2</v>
+      </c>
+      <c r="AI89" s="59">
+        <f t="shared" si="182"/>
+        <v>1.0327903345023997</v>
       </c>
     </row>
   </sheetData>
@@ -18664,10 +19353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:A86"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88:J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -18740,7 +19429,7 @@
         <v>93</v>
       </c>
       <c r="J2" s="47">
-        <f>(C2*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E2*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C2:H2)</f>
+        <f>(C2*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D2*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E2*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F2*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G2*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H2*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C2:H2)</f>
         <v>7.1062365591397834</v>
       </c>
     </row>
@@ -18774,7 +19463,7 @@
         <v>38</v>
       </c>
       <c r="J3" s="47">
-        <f>(C3*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D3*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E3*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F3*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G3*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H3*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C3:H3)</f>
+        <f>(C3*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D3*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E3*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F3*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G3*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H3*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C3:H3)</f>
         <v>7.4123684210526308</v>
       </c>
     </row>
@@ -18808,7 +19497,7 @@
         <v>81</v>
       </c>
       <c r="J4" s="47">
-        <f>(C4*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D4*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E4*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F4*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G4*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H4*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C4:H4)</f>
+        <f>(C4*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D4*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E4*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F4*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G4*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H4*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C4:H4)</f>
         <v>9.2016049382716059</v>
       </c>
     </row>
@@ -18842,7 +19531,7 @@
         <v>90</v>
       </c>
       <c r="J5" s="47">
-        <f>(C5*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D5*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E5*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F5*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G5*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H5*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C5:H5)</f>
+        <f>(C5*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D5*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E5*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F5*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G5*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H5*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C5:H5)</f>
         <v>8.8357777777777784</v>
       </c>
     </row>
@@ -18876,7 +19565,7 @@
         <v>94</v>
       </c>
       <c r="J6" s="47">
-        <f>(C6*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D6*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E6*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F6*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G6*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H6*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C6:H6)</f>
+        <f>(C6*VLOOKUP($C$1,OP!$A$59:$B$65,2,FALSE)+D6*VLOOKUP($D$1,OP!$A$59:$B$65,2,FALSE)+E6*VLOOKUP($E$1,OP!$A$59:$B$65,2,FALSE)+F6*VLOOKUP($F$1,OP!$A$59:$B$65,2,FALSE)+G6*VLOOKUP($G$1,OP!$A$59:$B$65,2,FALSE)+H6*VLOOKUP($H$1,OP!$A$59:$B$65,2,FALSE))/SUM(C6:H6)</f>
         <v>9.8862765957446808</v>
       </c>
     </row>
@@ -18910,7 +19599,7 @@
         <v>41</v>
       </c>
       <c r="J7" s="47">
-        <f>(C7*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D7*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E7*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F7*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G7*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H7*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C7:H7)</f>
+        <f>(C7*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D7*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E7*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F7*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G7*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H7*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C7:H7)</f>
         <v>10.65341463414634</v>
       </c>
     </row>
@@ -18944,7 +19633,7 @@
         <v>63</v>
       </c>
       <c r="J8" s="47">
-        <f>(C8*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D8*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E8*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F8*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G8*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H8*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C8:H8)</f>
+        <f>(C8*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D8*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E8*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F8*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G8*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H8*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C8:H8)</f>
         <v>11.008888888888889</v>
       </c>
     </row>
@@ -18978,7 +19667,7 @@
         <v>72</v>
       </c>
       <c r="J9" s="47">
-        <f>(C9*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D9*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E9*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F9*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G9*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H9*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C9:H9)</f>
+        <f>(C9*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D9*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E9*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F9*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G9*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H9*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C9:H9)</f>
         <v>12.317361111111111</v>
       </c>
     </row>
@@ -19012,7 +19701,7 @@
         <v>69</v>
       </c>
       <c r="J10" s="47">
-        <f>(C10*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D10*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E10*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F10*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G10*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H10*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C10:H10)</f>
+        <f>(C10*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D10*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E10*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F10*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G10*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H10*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C10:H10)</f>
         <v>11.958695652173912</v>
       </c>
     </row>
@@ -19046,7 +19735,7 @@
         <v>86</v>
       </c>
       <c r="J11" s="47">
-        <f>(C11*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D11*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E11*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F11*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G11*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H11*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C11:H11)</f>
+        <f>(C11*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D11*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E11*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F11*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G11*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H11*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C11:H11)</f>
         <v>11.538372093023256</v>
       </c>
     </row>
@@ -19080,7 +19769,7 @@
         <v>73</v>
       </c>
       <c r="J12" s="47">
-        <f>(C12*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D12*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E12*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F12*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G12*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H12*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C12:H12)</f>
+        <f>(C12*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D12*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E12*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F12*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G12*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H12*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C12:H12)</f>
         <v>11.79082191780822</v>
       </c>
     </row>
@@ -19114,7 +19803,7 @@
         <v>51</v>
       </c>
       <c r="J13" s="47">
-        <f>(C13*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D13*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E13*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F13*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G13*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H13*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C13:H13)</f>
+        <f>(C13*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D13*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E13*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F13*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G13*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H13*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C13:H13)</f>
         <v>11.26686274509804</v>
       </c>
     </row>
@@ -19148,7 +19837,7 @@
         <v>75</v>
       </c>
       <c r="J14" s="47">
-        <f>(C14*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D14*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E14*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F14*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G14*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H14*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C14:H14)</f>
+        <f>(C14*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D14*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E14*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F14*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G14*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H14*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C14:H14)</f>
         <v>10.407333333333332</v>
       </c>
     </row>
@@ -19182,7 +19871,7 @@
         <v>85</v>
       </c>
       <c r="J15" s="47">
-        <f>(C15*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D15*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E15*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F15*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G15*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H15*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C15:H15)</f>
+        <f>(C15*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D15*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E15*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F15*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G15*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H15*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C15:H15)</f>
         <v>12.336117647058822</v>
       </c>
     </row>
@@ -19216,7 +19905,7 @@
         <v>83</v>
       </c>
       <c r="J16" s="47">
-        <f>(C16*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D16*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E16*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F16*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G16*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H16*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C16:H16)</f>
+        <f>(C16*VLOOKUP($C$1,OP!$A$52:$B$58,2,FALSE)+D16*VLOOKUP($D$1,OP!$A$52:$B$58,2,FALSE)+E16*VLOOKUP($E$1,OP!$A$52:$B$58,2,FALSE)+F16*VLOOKUP($F$1,OP!$A$52:$B$58,2,FALSE)+G16*VLOOKUP($G$1,OP!$A$52:$B$58,2,FALSE)+H16*VLOOKUP($H$1,OP!$A$52:$B$58,2,FALSE))/SUM(C16:H16)</f>
         <v>12.719036144578311</v>
       </c>
     </row>
@@ -19250,7 +19939,7 @@
         <v>74</v>
       </c>
       <c r="J17" s="47">
-        <f>(C17*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D17*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E17*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F17*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G17*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H17*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C17:H17)</f>
+        <f>(C17*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D17*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E17*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F17*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G17*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H17*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C17:H17)</f>
         <v>12.701891891891892</v>
       </c>
     </row>
@@ -19284,7 +19973,7 @@
         <v>119</v>
       </c>
       <c r="J18" s="47">
-        <f>(C18*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D18*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E18*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F18*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G18*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H18*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C18:H18)</f>
+        <f>(C18*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D18*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E18*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F18*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G18*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H18*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C18:H18)</f>
         <v>13.471848739495798</v>
       </c>
     </row>
@@ -19318,7 +20007,7 @@
         <v>70</v>
       </c>
       <c r="J19" s="47">
-        <f>(C19*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D19*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E19*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F19*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G19*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H19*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C19:H19)</f>
+        <f>(C19*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D19*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E19*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F19*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G19*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H19*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C19:H19)</f>
         <v>12.774999999999999</v>
       </c>
     </row>
@@ -19352,7 +20041,7 @@
         <v>52</v>
       </c>
       <c r="J20" s="47">
-        <f>(C20*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D20*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E20*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F20*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G20*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H20*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C20:H20)</f>
+        <f>(C20*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D20*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E20*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F20*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G20*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H20*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C20:H20)</f>
         <v>11.37269230769231</v>
       </c>
     </row>
@@ -19386,7 +20075,7 @@
         <v>56</v>
       </c>
       <c r="J21" s="47">
-        <f>(C21*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D21*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E21*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F21*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G21*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H21*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C21:H21)</f>
+        <f>(C21*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D21*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E21*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F21*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G21*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H21*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C21:H21)</f>
         <v>13.873571428571429</v>
       </c>
     </row>
@@ -19420,7 +20109,7 @@
         <v>74</v>
       </c>
       <c r="J22" s="47">
-        <f>(C22*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D22*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E22*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F22*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G22*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H22*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C22:H22)</f>
+        <f>(C22*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D22*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E22*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F22*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G22*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H22*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C22:H22)</f>
         <v>13.749864864864865</v>
       </c>
     </row>
@@ -19454,7 +20143,7 @@
         <v>67</v>
       </c>
       <c r="J23" s="47">
-        <f>(C23*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D23*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E23*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F23*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G23*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H23*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C23:H23)</f>
+        <f>(C23*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D23*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E23*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F23*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G23*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H23*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C23:H23)</f>
         <v>14.991044776119404</v>
       </c>
     </row>
@@ -19488,7 +20177,7 @@
         <v>84</v>
       </c>
       <c r="J24" s="47">
-        <f>(C24*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D24*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E24*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F24*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G24*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H24*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C24:H24)</f>
+        <f>(C24*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D24*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E24*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F24*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G24*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H24*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C24:H24)</f>
         <v>14.623928571428573</v>
       </c>
     </row>
@@ -19522,7 +20211,7 @@
         <v>69</v>
       </c>
       <c r="J25" s="47">
-        <f>(C25*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D25*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E25*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F25*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G25*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H25*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C25:H25)</f>
+        <f>(C25*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D25*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E25*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F25*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G25*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H25*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C25:H25)</f>
         <v>13.701739130434783</v>
       </c>
     </row>
@@ -19556,7 +20245,7 @@
         <v>51</v>
       </c>
       <c r="J26" s="47">
-        <f>(C26*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D26*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E26*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F26*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G26*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H26*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C26:H26)</f>
+        <f>(C26*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D26*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E26*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F26*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G26*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H26*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C26:H26)</f>
         <v>15.005098039215687</v>
       </c>
     </row>
@@ -19590,7 +20279,7 @@
         <v>40</v>
       </c>
       <c r="J27" s="47">
-        <f>(C27*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D27*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E27*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F27*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G27*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H27*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C27:H27)</f>
+        <f>(C27*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D27*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E27*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F27*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G27*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H27*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C27:H27)</f>
         <v>14.773</v>
       </c>
     </row>
@@ -19624,7 +20313,7 @@
         <v>48</v>
       </c>
       <c r="J28" s="47">
-        <f>(C28*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D28*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E28*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F28*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G28*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H28*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C28:H28)</f>
+        <f>(C28*VLOOKUP($C$1,OP!$A$45:$B$51,2,FALSE)+D28*VLOOKUP($D$1,OP!$A$45:$B$51,2,FALSE)+E28*VLOOKUP($E$1,OP!$A$45:$B$51,2,FALSE)+F28*VLOOKUP($F$1,OP!$A$45:$B$51,2,FALSE)+G28*VLOOKUP($G$1,OP!$A$45:$B$51,2,FALSE)+H28*VLOOKUP($H$1,OP!$A$45:$B$51,2,FALSE))/SUM(C28:H28)</f>
         <v>12.647708333333334</v>
       </c>
     </row>
@@ -19658,7 +20347,7 @@
         <v>58</v>
       </c>
       <c r="J29" s="11">
-        <f>(C29*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D29*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E29*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F29*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G29*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H29*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C29:H29)</f>
+        <f>(C29*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D29*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E29*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F29*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G29*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H29*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C29:H29)</f>
         <v>13.190344827586209</v>
       </c>
     </row>
@@ -19692,7 +20381,7 @@
         <v>33</v>
       </c>
       <c r="J30" s="11">
-        <f>(C30*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D30*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E30*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F30*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G30*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H30*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C30:H30)</f>
+        <f>(C30*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D30*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E30*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F30*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G30*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H30*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C30:H30)</f>
         <v>14.081212121212122</v>
       </c>
     </row>
@@ -19726,7 +20415,7 @@
         <v>32</v>
       </c>
       <c r="J31" s="11">
-        <f>(C31*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D31*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E31*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F31*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G31*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H31*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C31:H31)</f>
+        <f>(C31*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D31*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E31*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F31*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G31*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H31*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C31:H31)</f>
         <v>13.164999999999999</v>
       </c>
     </row>
@@ -19760,7 +20449,7 @@
         <v>35</v>
       </c>
       <c r="J32" s="11">
-        <f>(C32*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D32*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E32*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F32*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G32*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H32*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C32:H32)</f>
+        <f>(C32*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D32*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E32*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F32*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G32*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H32*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C32:H32)</f>
         <v>12.799142857142854</v>
       </c>
     </row>
@@ -19794,7 +20483,7 @@
         <v>73</v>
       </c>
       <c r="J33" s="11">
-        <f>(C33*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D33*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E33*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F33*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G33*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H33*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C33:H33)</f>
+        <f>(C33*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D33*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E33*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F33*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G33*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H33*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C33:H33)</f>
         <v>13.504794520547945</v>
       </c>
     </row>
@@ -19828,7 +20517,7 @@
         <v>58</v>
       </c>
       <c r="J34" s="11">
-        <f>(C34*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D34*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E34*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F34*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G34*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H34*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C34:H34)</f>
+        <f>(C34*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D34*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E34*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F34*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G34*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H34*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C34:H34)</f>
         <v>12.611034482758622</v>
       </c>
     </row>
@@ -19862,7 +20551,7 @@
         <v>29</v>
       </c>
       <c r="J35" s="11">
-        <f>(C35*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D35*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E35*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F35*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G35*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H35*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C35:H35)</f>
+        <f>(C35*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D35*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E35*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F35*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G35*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H35*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C35:H35)</f>
         <v>12.230344827586206</v>
       </c>
     </row>
@@ -19896,7 +20585,7 @@
         <v>47</v>
       </c>
       <c r="J36" s="11">
-        <f>(C36*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D36*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E36*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F36*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G36*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H36*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C36:H36)</f>
+        <f>(C36*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D36*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E36*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F36*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G36*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H36*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C36:H36)</f>
         <v>13.969787234042551</v>
       </c>
     </row>
@@ -19930,7 +20619,7 @@
         <v>77</v>
       </c>
       <c r="J37" s="11">
-        <f>(C37*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D37*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E37*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F37*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G37*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H37*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C37:H37)</f>
+        <f>(C37*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D37*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E37*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F37*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G37*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H37*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C37:H37)</f>
         <v>13.64038961038961</v>
       </c>
     </row>
@@ -19964,7 +20653,7 @@
         <v>43</v>
       </c>
       <c r="J38" s="11">
-        <f>(C38*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D38*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E38*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F38*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G38*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H38*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C38:H38)</f>
+        <f>(C38*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D38*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E38*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F38*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G38*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H38*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C38:H38)</f>
         <v>14.050697674418604</v>
       </c>
     </row>
@@ -19998,7 +20687,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="11">
-        <f>(C39*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D39*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E39*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F39*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G39*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H39*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C39:H39)</f>
+        <f>(C39*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D39*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E39*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F39*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G39*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H39*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C39:H39)</f>
         <v>13.122</v>
       </c>
     </row>
@@ -20032,7 +20721,7 @@
         <v>24</v>
       </c>
       <c r="J40" s="11">
-        <f>(C40*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D40*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E40*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F40*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G40*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H40*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C40:H40)</f>
+        <f>(C40*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D40*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E40*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F40*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G40*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H40*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C40:H40)</f>
         <v>13.438333333333333</v>
       </c>
     </row>
@@ -20066,7 +20755,7 @@
         <v>24</v>
       </c>
       <c r="J41" s="11">
-        <f>(C41*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D41*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E41*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F41*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G41*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H41*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C41:H41)</f>
+        <f>(C41*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D41*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E41*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F41*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G41*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H41*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C41:H41)</f>
         <v>13.279166666666667</v>
       </c>
     </row>
@@ -20100,7 +20789,7 @@
         <v>24</v>
       </c>
       <c r="J42" s="11">
-        <f>(C42*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D42*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E42*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F42*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G42*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H42*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C42:H42)</f>
+        <f>(C42*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D42*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E42*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F42*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G42*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H42*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C42:H42)</f>
         <v>13.438333333333333</v>
       </c>
     </row>
@@ -20134,7 +20823,7 @@
         <v>47</v>
       </c>
       <c r="J43" s="11">
-        <f>(C43*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D43*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E43*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F43*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G43*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H43*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C43:H43)</f>
+        <f>(C43*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D43*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E43*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F43*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G43*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H43*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C43:H43)</f>
         <v>14.318936170212766</v>
       </c>
     </row>
@@ -20168,7 +20857,7 @@
         <v>33</v>
       </c>
       <c r="J44" s="11">
-        <f>(C44*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D44*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E44*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F44*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G44*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H44*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C44:H44)</f>
+        <f>(C44*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D44*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E44*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F44*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G44*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H44*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C44:H44)</f>
         <v>13.869393939393937</v>
       </c>
     </row>
@@ -20202,7 +20891,7 @@
         <v>38</v>
       </c>
       <c r="J45" s="11">
-        <f>(C45*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D45*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E45*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F45*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G45*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H45*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C45:H45)</f>
+        <f>(C45*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D45*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E45*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F45*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G45*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H45*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C45:H45)</f>
         <v>12.273421052631578</v>
       </c>
     </row>
@@ -20236,7 +20925,7 @@
         <v>20</v>
       </c>
       <c r="J46" s="11">
-        <f>(C46*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D46*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E46*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F46*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G46*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H46*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C46:H46)</f>
+        <f>(C46*VLOOKUP($C$1,OP!$A$38:$B$44,2,FALSE)+D46*VLOOKUP($D$1,OP!$A$38:$B$44,2,FALSE)+E46*VLOOKUP($E$1,OP!$A$38:$B$44,2,FALSE)+F46*VLOOKUP($F$1,OP!$A$38:$B$44,2,FALSE)+G46*VLOOKUP($G$1,OP!$A$38:$B$44,2,FALSE)+H46*VLOOKUP($H$1,OP!$A$38:$B$44,2,FALSE))/SUM(C46:H46)</f>
         <v>13.482000000000003</v>
       </c>
     </row>
@@ -20270,7 +20959,7 @@
         <v>45</v>
       </c>
       <c r="J47" s="11">
-        <f>(C47*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D47*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E47*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F47*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G47*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H47*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C47:H47)</f>
+        <f>(C47*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D47*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E47*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F47*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G47*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H47*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C47:H47)</f>
         <v>14.965333333333335</v>
       </c>
     </row>
@@ -20304,7 +20993,7 @@
         <v>41</v>
       </c>
       <c r="J48" s="11">
-        <f>(C48*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D48*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E48*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F48*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G48*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H48*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C48:H48)</f>
+        <f>(C48*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D48*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E48*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F48*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G48*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H48*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C48:H48)</f>
         <v>14.640975609756097</v>
       </c>
     </row>
@@ -20338,7 +21027,7 @@
         <v>30</v>
       </c>
       <c r="J49" s="11">
-        <f>(C49*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D49*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E49*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F49*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G49*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H49*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C49:H49)</f>
+        <f>(C49*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D49*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E49*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F49*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G49*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H49*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C49:H49)</f>
         <v>13.525</v>
       </c>
     </row>
@@ -20372,7 +21061,7 @@
         <v>39</v>
       </c>
       <c r="J50" s="11">
-        <f>(C50*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D50*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E50*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F50*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G50*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H50*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C50:H50)</f>
+        <f>(C50*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D50*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E50*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F50*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G50*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H50*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C50:H50)</f>
         <v>13.716666666666665</v>
       </c>
     </row>
@@ -20406,7 +21095,7 @@
         <v>33</v>
       </c>
       <c r="J51" s="11">
-        <f>(C51*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D51*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E51*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F51*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G51*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H51*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C51:H51)</f>
+        <f>(C51*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D51*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E51*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F51*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G51*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H51*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C51:H51)</f>
         <v>14.153030303030302</v>
       </c>
     </row>
@@ -20440,7 +21129,7 @@
         <v>33</v>
       </c>
       <c r="J52" s="11">
-        <f>(C52*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D52*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E52*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F52*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G52*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H52*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C52:H52)</f>
+        <f>(C52*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D52*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E52*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F52*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G52*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H52*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C52:H52)</f>
         <v>12.247272727272726</v>
       </c>
     </row>
@@ -20474,7 +21163,7 @@
         <v>27</v>
       </c>
       <c r="J53" s="11">
-        <f>(C53*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D53*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E53*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F53*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G53*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H53*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C53:H53)</f>
+        <f>(C53*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D53*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E53*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F53*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G53*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H53*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C53:H53)</f>
         <v>13.40185185185185</v>
       </c>
     </row>
@@ -20508,7 +21197,7 @@
         <v>52</v>
       </c>
       <c r="J54" s="11">
-        <f>(C54*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D54*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E54*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F54*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G54*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H54*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C54:H54)</f>
+        <f>(C54*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D54*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E54*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F54*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G54*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H54*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C54:H54)</f>
         <v>12.881538461538462</v>
       </c>
     </row>
@@ -20542,7 +21231,7 @@
         <v>50</v>
       </c>
       <c r="J55" s="11">
-        <f>(C55*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D55*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E55*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F55*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G55*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H55*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C55:H55)</f>
+        <f>(C55*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D55*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E55*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F55*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G55*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H55*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C55:H55)</f>
         <v>13.323400000000001</v>
       </c>
     </row>
@@ -20576,7 +21265,7 @@
         <v>29</v>
       </c>
       <c r="J56" s="11">
-        <f>(C56*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D56*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E56*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F56*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G56*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H56*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C56:H56)</f>
+        <f>(C56*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D56*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E56*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F56*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G56*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H56*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C56:H56)</f>
         <v>13.320344827586208</v>
       </c>
     </row>
@@ -20610,7 +21299,7 @@
         <v>57</v>
       </c>
       <c r="J57" s="11">
-        <f>(C57*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D57*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E57*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F57*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G57*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H57*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C57:H57)</f>
+        <f>(C57*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D57*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E57*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F57*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G57*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H57*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C57:H57)</f>
         <v>11.868771929824561</v>
       </c>
     </row>
@@ -20644,7 +21333,7 @@
         <v>34</v>
       </c>
       <c r="J58" s="11">
-        <f>(C58*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D58*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E58*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F58*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G58*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H58*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C58:H58)</f>
+        <f>(C58*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D58*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E58*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F58*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G58*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H58*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C58:H58)</f>
         <v>12.511470588235293</v>
       </c>
     </row>
@@ -20678,7 +21367,7 @@
         <v>53</v>
       </c>
       <c r="J59" s="11">
-        <f>(C59*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D59*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E59*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F59*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G59*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H59*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C59:H59)</f>
+        <f>(C59*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D59*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E59*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F59*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G59*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H59*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C59:H59)</f>
         <v>13.196981132075473</v>
       </c>
     </row>
@@ -20712,7 +21401,7 @@
         <v>66</v>
       </c>
       <c r="J60" s="11">
-        <f>(C60*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D60*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E60*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F60*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G60*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H60*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C60:H60)</f>
+        <f>(C60*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D60*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E60*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F60*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G60*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H60*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C60:H60)</f>
         <v>13.417272727272726</v>
       </c>
     </row>
@@ -20778,7 +21467,7 @@
         <v>66</v>
       </c>
       <c r="J62" s="11">
-        <f>(C62*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D62*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E62*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F62*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G62*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H62*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C62:H62)</f>
+        <f>(C62*VLOOKUP($C$1,OP!$A$31:$B$37,2,FALSE)+D62*VLOOKUP($D$1,OP!$A$31:$B$37,2,FALSE)+E62*VLOOKUP($E$1,OP!$A$31:$B$37,2,FALSE)+F62*VLOOKUP($F$1,OP!$A$31:$B$37,2,FALSE)+G62*VLOOKUP($G$1,OP!$A$31:$B$37,2,FALSE)+H62*VLOOKUP($H$1,OP!$A$31:$B$37,2,FALSE))/SUM(C62:H62)</f>
         <v>13.417272727272726</v>
       </c>
     </row>
@@ -20812,7 +21501,7 @@
         <v>64</v>
       </c>
       <c r="J63" s="11">
-        <f>(C63*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D63*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E63*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F63*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G63*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H63*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C63:H63)</f>
+        <f>(C63*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D63*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E63*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F63*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G63*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H63*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C63:H63)</f>
         <v>15.414969104075293</v>
       </c>
     </row>
@@ -20846,7 +21535,7 @@
         <v>37</v>
       </c>
       <c r="J64" s="11">
-        <f>(C64*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D64*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E64*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F64*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G64*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H64*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C64:H64)</f>
+        <f>(C64*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D64*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E64*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F64*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G64*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H64*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C64:H64)</f>
         <v>13.738015647226174</v>
       </c>
     </row>
@@ -20880,7 +21569,7 @@
         <v>5</v>
       </c>
       <c r="J65" s="11">
-        <f>(C65*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D65*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E65*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F65*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G65*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H65*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C65:H65)</f>
+        <f>(C65*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D65*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E65*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F65*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G65*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H65*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C65:H65)</f>
         <v>14.144736842105264</v>
       </c>
     </row>
@@ -20914,7 +21603,7 @@
         <v>21</v>
       </c>
       <c r="J66" s="11">
-        <f>(C66*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D66*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E66*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F66*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G66*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H66*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C66:H66)</f>
+        <f>(C66*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D66*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E66*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F66*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G66*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H66*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C66:H66)</f>
         <v>15.447447612085769</v>
       </c>
     </row>
@@ -20948,7 +21637,7 @@
         <v>29</v>
       </c>
       <c r="J67" s="11">
-        <f>(C67*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D67*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E67*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F67*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G67*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H67*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C67:H67)</f>
+        <f>(C67*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D67*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E67*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F67*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G67*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H67*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C67:H67)</f>
         <v>14.698407567049811</v>
       </c>
     </row>
@@ -20982,7 +21671,7 @@
         <v>31</v>
       </c>
       <c r="J68" s="11">
-        <f>(C68*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D68*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E68*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F68*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G68*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H68*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C68:H68)</f>
+        <f>(C68*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D68*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E68*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F68*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G68*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H68*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C68:H68)</f>
         <v>13.777215973401246</v>
       </c>
     </row>
@@ -21016,7 +21705,7 @@
         <v>48</v>
       </c>
       <c r="J69" s="11">
-        <f>(C69*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D69*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E69*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F69*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G69*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H69*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C69:H69)</f>
+        <f>(C69*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D69*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E69*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F69*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G69*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H69*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C69:H69)</f>
         <v>13.38032102826511</v>
       </c>
     </row>
@@ -21050,7 +21739,7 @@
         <v>31</v>
       </c>
       <c r="J70" s="11">
-        <f>(C70*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D70*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E70*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F70*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G70*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H70*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C70:H70)</f>
+        <f>(C70*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D70*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E70*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F70*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G70*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H70*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C70:H70)</f>
         <v>13.777215973401246</v>
       </c>
     </row>
@@ -21084,7 +21773,7 @@
         <v>45</v>
       </c>
       <c r="J71" s="11">
-        <f>(C71*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D71*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E71*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F71*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G71*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H71*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C71:H71)</f>
+        <f>(C71*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D71*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E71*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F71*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G71*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H71*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C71:H71)</f>
         <v>15.632973927875243</v>
       </c>
     </row>
@@ -21118,7 +21807,7 @@
         <v>67</v>
       </c>
       <c r="J72" s="11">
-        <f>(C72*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D72*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E72*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F72*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G72*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H72*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C72:H72)</f>
+        <f>(C72*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D72*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E72*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F72*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G72*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H72*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C72:H72)</f>
         <v>15.176211322772104</v>
       </c>
     </row>
@@ -21152,7 +21841,7 @@
         <v>38</v>
       </c>
       <c r="J73" s="11">
-        <f>(C73*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E73*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C73:H73)</f>
+        <f>(C73*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D73*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E73*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F73*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G73*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H73*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C73:H73)</f>
         <v>16.690074349799939</v>
       </c>
     </row>
@@ -21186,7 +21875,7 @@
         <v>40</v>
       </c>
       <c r="J74" s="11">
-        <f>(C74*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E74*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C74:H74)</f>
+        <f>(C74*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D74*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E74*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F74*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G74*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H74*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C74:H74)</f>
         <v>15.830891812865499</v>
       </c>
     </row>
@@ -21220,7 +21909,7 @@
         <v>38</v>
       </c>
       <c r="J75" s="11">
-        <f>(C75*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E75*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C75:H75)</f>
+        <f>(C75*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D75*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E75*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F75*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G75*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H75*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C75:H75)</f>
         <v>15.258149142043706</v>
       </c>
     </row>
@@ -21254,7 +21943,7 @@
         <v>45</v>
       </c>
       <c r="J76" s="11">
-        <f>(C76*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E76*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C76:H76)</f>
+        <f>(C76*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D76*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E76*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F76*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G76*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H76*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C76:H76)</f>
         <v>14.714600795971414</v>
       </c>
     </row>
@@ -21288,7 +21977,7 @@
         <v>46</v>
       </c>
       <c r="J77" s="11">
-        <f>(C77*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E77*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C77:H77)</f>
+        <f>(C77*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D77*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E77*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F77*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G77*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H77*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C77:H77)</f>
         <v>15.666122393846935</v>
       </c>
     </row>
@@ -21322,7 +22011,7 @@
         <v>57</v>
       </c>
       <c r="J78" s="11">
-        <f>(C78*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D78*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E78*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F78*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G78*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H78*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C78:H78)</f>
+        <f>(C78*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D78*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E78*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F78*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G78*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H78*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C78:H78)</f>
         <v>14.741700330871039</v>
       </c>
     </row>
@@ -21356,7 +22045,7 @@
         <v>56</v>
       </c>
       <c r="J79" s="11">
-        <f>(C79*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D79*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E79*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F79*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G79*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H79*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C79:H79)</f>
+        <f>(C79*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D79*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E79*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F79*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G79*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H79*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C79:H79)</f>
         <v>14.663393509816206</v>
       </c>
     </row>
@@ -21390,7 +22079,7 @@
         <v>54</v>
       </c>
       <c r="J80" s="11">
-        <f>(C80*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D80*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E80*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F80*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G80*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H80*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C80:H80)</f>
+        <f>(C80*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D80*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E80*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F80*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G80*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H80*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C80:H80)</f>
         <v>15.356992500541478</v>
       </c>
     </row>
@@ -21424,7 +22113,7 @@
         <v>68</v>
       </c>
       <c r="J81" s="11">
-        <f>(C81*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D81*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E81*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F81*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G81*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H81*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C81:H81)</f>
+        <f>(C81*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D81*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E81*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F81*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G81*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H81*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C81:H81)</f>
         <v>14.555771091331271</v>
       </c>
     </row>
@@ -21458,7 +22147,7 @@
         <v>68</v>
       </c>
       <c r="J82" s="11">
-        <f>(C82*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D82*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E82*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F82*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G82*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H82*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C82:H82)</f>
+        <f>(C82*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D82*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E82*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F82*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G82*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H82*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C82:H82)</f>
         <v>15.100360122119024</v>
       </c>
     </row>
@@ -21492,7 +22181,7 @@
         <v>84</v>
       </c>
       <c r="J83" s="11">
-        <f>(C83*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D83*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E83*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F83*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G83*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H83*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C83:H83)</f>
+        <f>(C83*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D83*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E83*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F83*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G83*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H83*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C83:H83)</f>
         <v>14.899068852687273</v>
       </c>
     </row>
@@ -21526,7 +22215,7 @@
         <v>73</v>
       </c>
       <c r="J84" s="11">
-        <f>(C84*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D84*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E84*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F84*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G84*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H84*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C84:H84)</f>
+        <f>(C84*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D84*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E84*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F84*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G84*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H84*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C84:H84)</f>
         <v>15.951802701674277</v>
       </c>
     </row>
@@ -21560,7 +22249,7 @@
         <v>81</v>
       </c>
       <c r="J85" s="11">
-        <f>(C85*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D85*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E85*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F85*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G85*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H85*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C85:H85)</f>
+        <f>(C85*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D85*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E85*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F85*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G85*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H85*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C85:H85)</f>
         <v>15.913511885423436</v>
       </c>
     </row>
@@ -21594,8 +22283,178 @@
         <v>54</v>
       </c>
       <c r="J86" s="11">
-        <f>(C86*VLOOKUP($C$1,OP!$A$17:$B$23,2,FALSE)+D86*VLOOKUP($D$1,OP!$A$17:$B$23,2,FALSE)+E86*VLOOKUP($E$1,OP!$A$17:$B$23,2,FALSE)+F86*VLOOKUP($F$1,OP!$A$17:$B$23,2,FALSE)+G86*VLOOKUP($G$1,OP!$A$17:$B$23,2,FALSE)+H86*VLOOKUP($H$1,OP!$A$17:$B$23,2,FALSE))/SUM(C86:H86)</f>
+        <f>(C86*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D86*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E86*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F86*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G86*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H86*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C86:H86)</f>
         <v>14.989051670457009</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="52">
+        <v>2024</v>
+      </c>
+      <c r="B87" s="52">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>37</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>5</v>
+      </c>
+      <c r="G87">
+        <v>11</v>
+      </c>
+      <c r="H87">
+        <v>7</v>
+      </c>
+      <c r="I87">
+        <f>SUM(C87:H87)</f>
+        <v>61</v>
+      </c>
+      <c r="J87" s="11">
+        <f>(C87*VLOOKUP($C$1,OP!$A$24:$B$30,2,FALSE)+D87*VLOOKUP($D$1,OP!$A$24:$B$30,2,FALSE)+E87*VLOOKUP($E$1,OP!$A$24:$B$30,2,FALSE)+F87*VLOOKUP($F$1,OP!$A$24:$B$30,2,FALSE)+G87*VLOOKUP($G$1,OP!$A$24:$B$30,2,FALSE)+H87*VLOOKUP($H$1,OP!$A$24:$B$30,2,FALSE))/SUM(C87:H87)</f>
+        <v>14.212922119164029</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="52">
+        <v>2024</v>
+      </c>
+      <c r="B88" s="52">
+        <v>8</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>35</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>5</v>
+      </c>
+      <c r="H88">
+        <v>7</v>
+      </c>
+      <c r="I88">
+        <f>SUM(C88:H88)</f>
+        <v>48</v>
+      </c>
+      <c r="J88" s="11">
+        <f>(C88*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D88*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+E88*VLOOKUP($E$1,OP!$A$18:$B$23,2,FALSE)+F88*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G88*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H88*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C88:H88)</f>
+        <v>14.788333333333332</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="52">
+        <v>2024</v>
+      </c>
+      <c r="B89" s="52">
+        <v>9</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>29</v>
+      </c>
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>11</v>
+      </c>
+      <c r="H89">
+        <v>4</v>
+      </c>
+      <c r="I89">
+        <f>SUM(C89:H89)</f>
+        <v>49</v>
+      </c>
+      <c r="J89" s="11">
+        <f>(C89*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D89*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+E89*VLOOKUP($E$1,OP!$A$18:$B$23,2,FALSE)+F89*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G89*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H89*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C89:H89)</f>
+        <v>16.593877551020409</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="52">
+        <v>2024</v>
+      </c>
+      <c r="B90" s="52">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>24</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>12</v>
+      </c>
+      <c r="H90">
+        <v>9</v>
+      </c>
+      <c r="I90">
+        <f>SUM(C90:H90)</f>
+        <v>50</v>
+      </c>
+      <c r="J90" s="11">
+        <f>(C90*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D90*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+E90*VLOOKUP($E$1,OP!$A$18:$B$23,2,FALSE)+F90*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G90*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H90*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C90:H90)</f>
+        <v>15.158200000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="52">
+        <v>2024</v>
+      </c>
+      <c r="B91" s="52">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>21</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>6</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <f>SUM(C91:H91)</f>
+        <v>29</v>
+      </c>
+      <c r="J91" s="11">
+        <f>(C91*VLOOKUP($C$1,OP!$A$18:$B$23,2,FALSE)+D91*VLOOKUP($D$1,OP!$A$18:$B$23,2,FALSE)+E91*VLOOKUP($E$1,OP!$A$18:$B$23,2,FALSE)+F91*VLOOKUP($F$1,OP!$A$18:$B$23,2,FALSE)+G91*VLOOKUP($G$1,OP!$A$18:$B$23,2,FALSE)+H91*VLOOKUP($H$1,OP!$A$18:$B$23,2,FALSE))/SUM(C91:H91)</f>
+        <v>17.372068965517244</v>
       </c>
     </row>
   </sheetData>
@@ -21608,10 +22467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6335AA81-92E1-4191-98F5-D9E75D89EE86}">
-  <dimension ref="A1:J357"/>
+  <dimension ref="A1:J382"/>
   <sheetViews>
-    <sheetView topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="J357" sqref="J357"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="H382" sqref="H382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -33383,6 +34242,831 @@
         <v>8</v>
       </c>
     </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>2024</v>
+      </c>
+      <c r="B358">
+        <v>7</v>
+      </c>
+      <c r="C358" t="s">
+        <v>57</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358">
+        <v>5</v>
+      </c>
+      <c r="F358">
+        <v>0</v>
+      </c>
+      <c r="G358">
+        <v>0</v>
+      </c>
+      <c r="H358">
+        <v>0</v>
+      </c>
+      <c r="I358">
+        <v>1</v>
+      </c>
+      <c r="J358">
+        <f t="shared" ref="J358:J362" si="69">SUM(D358:I358)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>2024</v>
+      </c>
+      <c r="B359">
+        <v>7</v>
+      </c>
+      <c r="C359" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+      <c r="E359">
+        <v>15</v>
+      </c>
+      <c r="F359">
+        <v>0</v>
+      </c>
+      <c r="G359">
+        <v>1</v>
+      </c>
+      <c r="H359">
+        <v>1</v>
+      </c>
+      <c r="I359">
+        <v>0</v>
+      </c>
+      <c r="J359">
+        <f t="shared" si="69"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>2024</v>
+      </c>
+      <c r="B360">
+        <v>7</v>
+      </c>
+      <c r="C360" t="s">
+        <v>60</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360">
+        <v>5</v>
+      </c>
+      <c r="F360">
+        <v>0</v>
+      </c>
+      <c r="G360">
+        <v>1</v>
+      </c>
+      <c r="H360">
+        <v>1</v>
+      </c>
+      <c r="I360">
+        <v>0</v>
+      </c>
+      <c r="J360">
+        <f t="shared" si="69"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>2024</v>
+      </c>
+      <c r="B361">
+        <v>7</v>
+      </c>
+      <c r="C361" t="s">
+        <v>69</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361">
+        <v>8</v>
+      </c>
+      <c r="F361">
+        <v>1</v>
+      </c>
+      <c r="G361">
+        <v>9</v>
+      </c>
+      <c r="H361">
+        <v>3</v>
+      </c>
+      <c r="I361">
+        <v>6</v>
+      </c>
+      <c r="J361">
+        <f t="shared" si="69"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>2024</v>
+      </c>
+      <c r="B362">
+        <v>7</v>
+      </c>
+      <c r="C362" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>4</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+      <c r="G362">
+        <v>0</v>
+      </c>
+      <c r="H362">
+        <v>0</v>
+      </c>
+      <c r="I362">
+        <v>0</v>
+      </c>
+      <c r="J362">
+        <f t="shared" si="69"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>2024</v>
+      </c>
+      <c r="B363">
+        <v>8</v>
+      </c>
+      <c r="C363" t="s">
+        <v>57</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>3</v>
+      </c>
+      <c r="F363">
+        <v>0</v>
+      </c>
+      <c r="G363">
+        <v>0</v>
+      </c>
+      <c r="H363">
+        <v>0</v>
+      </c>
+      <c r="I363">
+        <v>1</v>
+      </c>
+      <c r="J363">
+        <f t="shared" ref="J363:J367" si="70">SUM(D363:I363)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>2024</v>
+      </c>
+      <c r="B364">
+        <v>8</v>
+      </c>
+      <c r="C364" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>13</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+      <c r="G364">
+        <v>0</v>
+      </c>
+      <c r="H364">
+        <v>0</v>
+      </c>
+      <c r="I364">
+        <v>2</v>
+      </c>
+      <c r="J364">
+        <f t="shared" si="70"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>2024</v>
+      </c>
+      <c r="B365">
+        <v>8</v>
+      </c>
+      <c r="C365" t="s">
+        <v>60</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>10</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+      <c r="G365">
+        <v>3</v>
+      </c>
+      <c r="H365">
+        <v>0</v>
+      </c>
+      <c r="I365">
+        <v>4</v>
+      </c>
+      <c r="J365">
+        <f t="shared" si="70"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>2024</v>
+      </c>
+      <c r="B366">
+        <v>8</v>
+      </c>
+      <c r="C366" t="s">
+        <v>69</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>4</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+      <c r="G366">
+        <v>1</v>
+      </c>
+      <c r="H366">
+        <v>0</v>
+      </c>
+      <c r="I366">
+        <v>0</v>
+      </c>
+      <c r="J366">
+        <f t="shared" si="70"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>2024</v>
+      </c>
+      <c r="B367">
+        <v>8</v>
+      </c>
+      <c r="C367" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>5</v>
+      </c>
+      <c r="F367">
+        <v>1</v>
+      </c>
+      <c r="G367">
+        <v>1</v>
+      </c>
+      <c r="H367">
+        <v>0</v>
+      </c>
+      <c r="I367">
+        <v>0</v>
+      </c>
+      <c r="J367">
+        <f t="shared" si="70"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>2024</v>
+      </c>
+      <c r="B368">
+        <v>9</v>
+      </c>
+      <c r="C368" t="s">
+        <v>57</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>1</v>
+      </c>
+      <c r="F368">
+        <v>0</v>
+      </c>
+      <c r="G368">
+        <v>5</v>
+      </c>
+      <c r="H368">
+        <v>0</v>
+      </c>
+      <c r="I368">
+        <v>0</v>
+      </c>
+      <c r="J368">
+        <f t="shared" ref="J368:J372" si="71">SUM(D368:I368)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>2024</v>
+      </c>
+      <c r="B369">
+        <v>9</v>
+      </c>
+      <c r="C369" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>7</v>
+      </c>
+      <c r="F369">
+        <v>2</v>
+      </c>
+      <c r="G369">
+        <v>3</v>
+      </c>
+      <c r="H369">
+        <v>1</v>
+      </c>
+      <c r="I369">
+        <v>2</v>
+      </c>
+      <c r="J369">
+        <f t="shared" si="71"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>2024</v>
+      </c>
+      <c r="B370">
+        <v>9</v>
+      </c>
+      <c r="C370" t="s">
+        <v>60</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370">
+        <v>10</v>
+      </c>
+      <c r="F370">
+        <v>0</v>
+      </c>
+      <c r="G370">
+        <v>2</v>
+      </c>
+      <c r="H370">
+        <v>0</v>
+      </c>
+      <c r="I370">
+        <v>1</v>
+      </c>
+      <c r="J370">
+        <f t="shared" si="71"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>2024</v>
+      </c>
+      <c r="B371">
+        <v>9</v>
+      </c>
+      <c r="C371" t="s">
+        <v>69</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>10</v>
+      </c>
+      <c r="F371">
+        <v>0</v>
+      </c>
+      <c r="G371">
+        <v>1</v>
+      </c>
+      <c r="H371">
+        <v>0</v>
+      </c>
+      <c r="I371">
+        <v>1</v>
+      </c>
+      <c r="J371">
+        <f t="shared" si="71"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>2024</v>
+      </c>
+      <c r="B372">
+        <v>9</v>
+      </c>
+      <c r="C372" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D372">
+        <v>0</v>
+      </c>
+      <c r="E372">
+        <v>1</v>
+      </c>
+      <c r="F372">
+        <v>1</v>
+      </c>
+      <c r="G372">
+        <v>0</v>
+      </c>
+      <c r="H372">
+        <v>1</v>
+      </c>
+      <c r="I372">
+        <v>0</v>
+      </c>
+      <c r="J372">
+        <f t="shared" si="71"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>2024</v>
+      </c>
+      <c r="B373">
+        <v>10</v>
+      </c>
+      <c r="C373" t="s">
+        <v>57</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373">
+        <v>3</v>
+      </c>
+      <c r="F373">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>0</v>
+      </c>
+      <c r="H373">
+        <v>0</v>
+      </c>
+      <c r="I373">
+        <v>0</v>
+      </c>
+      <c r="J373">
+        <f t="shared" ref="J373:J377" si="72">SUM(D373:I373)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>2024</v>
+      </c>
+      <c r="B374">
+        <v>10</v>
+      </c>
+      <c r="C374" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374">
+        <v>4</v>
+      </c>
+      <c r="F374">
+        <v>0</v>
+      </c>
+      <c r="G374">
+        <v>4</v>
+      </c>
+      <c r="H374">
+        <v>0</v>
+      </c>
+      <c r="I374">
+        <v>1</v>
+      </c>
+      <c r="J374">
+        <f t="shared" si="72"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>2024</v>
+      </c>
+      <c r="B375">
+        <v>10</v>
+      </c>
+      <c r="C375" t="s">
+        <v>60</v>
+      </c>
+      <c r="D375">
+        <v>0</v>
+      </c>
+      <c r="E375">
+        <v>4</v>
+      </c>
+      <c r="F375">
+        <v>0</v>
+      </c>
+      <c r="G375">
+        <v>6</v>
+      </c>
+      <c r="H375">
+        <v>3</v>
+      </c>
+      <c r="I375">
+        <v>5</v>
+      </c>
+      <c r="J375">
+        <f t="shared" si="72"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>2024</v>
+      </c>
+      <c r="B376">
+        <v>10</v>
+      </c>
+      <c r="C376" t="s">
+        <v>69</v>
+      </c>
+      <c r="D376">
+        <v>1</v>
+      </c>
+      <c r="E376">
+        <v>12</v>
+      </c>
+      <c r="F376">
+        <v>1</v>
+      </c>
+      <c r="G376">
+        <v>2</v>
+      </c>
+      <c r="H376">
+        <v>0</v>
+      </c>
+      <c r="I376">
+        <v>3</v>
+      </c>
+      <c r="J376">
+        <f t="shared" si="72"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>2024</v>
+      </c>
+      <c r="B377">
+        <v>10</v>
+      </c>
+      <c r="C377" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>1</v>
+      </c>
+      <c r="F377">
+        <v>0</v>
+      </c>
+      <c r="G377">
+        <v>0</v>
+      </c>
+      <c r="H377">
+        <v>0</v>
+      </c>
+      <c r="I377">
+        <v>0</v>
+      </c>
+      <c r="J377">
+        <f t="shared" si="72"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>2024</v>
+      </c>
+      <c r="B378">
+        <v>11</v>
+      </c>
+      <c r="C378" t="s">
+        <v>57</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>2</v>
+      </c>
+      <c r="F378">
+        <v>0</v>
+      </c>
+      <c r="G378">
+        <v>4</v>
+      </c>
+      <c r="H378">
+        <v>1</v>
+      </c>
+      <c r="I378">
+        <v>0</v>
+      </c>
+      <c r="J378">
+        <f t="shared" ref="J378:J382" si="73">SUM(D378:I378)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>2024</v>
+      </c>
+      <c r="B379">
+        <v>11</v>
+      </c>
+      <c r="C379" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>5</v>
+      </c>
+      <c r="F379">
+        <v>0</v>
+      </c>
+      <c r="G379">
+        <v>1</v>
+      </c>
+      <c r="H379">
+        <v>0</v>
+      </c>
+      <c r="I379">
+        <v>0</v>
+      </c>
+      <c r="J379">
+        <f t="shared" si="73"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>2024</v>
+      </c>
+      <c r="B380">
+        <v>11</v>
+      </c>
+      <c r="C380" t="s">
+        <v>60</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380">
+        <v>7</v>
+      </c>
+      <c r="F380">
+        <v>1</v>
+      </c>
+      <c r="G380">
+        <v>1</v>
+      </c>
+      <c r="H380">
+        <v>0</v>
+      </c>
+      <c r="I380">
+        <v>0</v>
+      </c>
+      <c r="J380">
+        <f t="shared" si="73"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>2024</v>
+      </c>
+      <c r="B381">
+        <v>11</v>
+      </c>
+      <c r="C381" t="s">
+        <v>69</v>
+      </c>
+      <c r="D381">
+        <v>0</v>
+      </c>
+      <c r="E381">
+        <v>2</v>
+      </c>
+      <c r="F381">
+        <v>0</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+      <c r="H381">
+        <v>0</v>
+      </c>
+      <c r="I381">
+        <v>0</v>
+      </c>
+      <c r="J381">
+        <f t="shared" si="73"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>2024</v>
+      </c>
+      <c r="B382">
+        <v>11</v>
+      </c>
+      <c r="C382" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382">
+        <v>5</v>
+      </c>
+      <c r="F382">
+        <v>0</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+      <c r="H382">
+        <v>0</v>
+      </c>
+      <c r="I382">
+        <v>0</v>
+      </c>
+      <c r="J382">
+        <f t="shared" si="73"/>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -33393,19 +35077,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EB2B5E-69B9-4E17-A8DC-DBA424D12F80}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G9"/>
+      <selection activeCell="B10" sqref="B10:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -33578,26 +35261,141 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0</v>
+      </c>
+      <c r="C10" s="13">
+        <v>37</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>5</v>
+      </c>
+      <c r="F10" s="13">
+        <v>11</v>
+      </c>
+      <c r="G10" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13">
+        <v>35</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>5</v>
+      </c>
+      <c r="G11" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0</v>
+      </c>
+      <c r="C12" s="13">
+        <v>29</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13">
+        <v>11</v>
+      </c>
+      <c r="G12" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13">
+        <v>24</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="13">
+        <v>12</v>
+      </c>
+      <c r="G13" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>11</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <v>21</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="13">
-        <v>0</v>
-      </c>
-      <c r="C10" s="13">
-        <v>248</v>
-      </c>
-      <c r="D10" s="13">
-        <v>31</v>
-      </c>
-      <c r="E10" s="13">
-        <v>29</v>
-      </c>
-      <c r="F10" s="13">
-        <v>93</v>
-      </c>
-      <c r="G10" s="13">
-        <v>27</v>
+      <c r="B15" s="13">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13">
+        <v>394</v>
+      </c>
+      <c r="D15" s="13">
+        <v>38</v>
+      </c>
+      <c r="E15" s="13">
+        <v>40</v>
+      </c>
+      <c r="F15" s="13">
+        <v>138</v>
+      </c>
+      <c r="G15" s="13">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -33607,10 +35405,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B23"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -33737,7 +35535,7 @@
         <v>24</v>
       </c>
       <c r="B17" s="60" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -33745,7 +35543,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="5">
-        <v>13.478947368421053</v>
+        <v>14.32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -33753,7 +35551,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5">
-        <v>14.144736842105264</v>
+        <v>15.66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -33761,7 +35559,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="5">
-        <v>19.183333333333334</v>
+        <v>20.68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -33769,7 +35567,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="5">
-        <v>18.605555555555554</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -33777,7 +35575,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="5">
-        <v>19.700000000000003</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33785,7 +35583,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="7">
-        <v>2.1031249999999995</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33793,7 +35591,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -33801,7 +35599,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="5">
-        <v>12.39</v>
+        <v>13.478947368421053</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -33809,7 +35607,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="5">
-        <v>14.07</v>
+        <v>14.144736842105264</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -33817,7 +35615,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="5">
-        <v>20.02</v>
+        <v>19.183333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -33825,7 +35623,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="5">
-        <v>10.69</v>
+        <v>18.605555555555554</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -33833,7 +35631,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="5">
-        <v>17.88</v>
+        <v>19.700000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33841,7 +35639,7 @@
         <v>20</v>
       </c>
       <c r="B30" s="7">
-        <v>2.69</v>
+        <v>2.1031249999999995</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33849,7 +35647,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="60" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -33857,7 +35655,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="5">
-        <v>10</v>
+        <v>12.39</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -33865,7 +35663,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="5">
-        <v>13.11</v>
+        <v>14.07</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -33873,7 +35671,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="5">
-        <v>18.84</v>
+        <v>20.02</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -33881,7 +35679,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="5">
-        <v>9.5299999999999994</v>
+        <v>10.69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -33889,7 +35687,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="5">
-        <v>16.93</v>
+        <v>17.88</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33897,15 +35695,15 @@
         <v>20</v>
       </c>
       <c r="B37" s="7">
-        <v>4.55</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>70</v>
+      <c r="B38" s="60" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -33921,7 +35719,7 @@
         <v>16</v>
       </c>
       <c r="B40" s="5">
-        <v>12.48</v>
+        <v>13.11</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -33929,7 +35727,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="5">
-        <v>17.7</v>
+        <v>18.84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -33937,7 +35735,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="5">
-        <v>9.61</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -33945,7 +35743,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="5">
-        <v>18.64</v>
+        <v>16.93</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33953,7 +35751,7 @@
         <v>20</v>
       </c>
       <c r="B44" s="7">
-        <v>2.48</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -33961,7 +35759,7 @@
         <v>24</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -33969,7 +35767,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="5">
-        <v>9.8000000000000007</v>
+        <v>10</v>
       </c>
       <c r="C46" s="11"/>
     </row>
@@ -33978,7 +35776,7 @@
         <v>16</v>
       </c>
       <c r="B47" s="5">
-        <v>13.02</v>
+        <v>12.48</v>
       </c>
       <c r="C47" s="11"/>
     </row>
@@ -33987,7 +35785,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="5">
-        <v>16.28</v>
+        <v>17.7</v>
       </c>
       <c r="C48" s="11"/>
     </row>
@@ -33996,7 +35794,7 @@
         <v>21</v>
       </c>
       <c r="B49" s="5">
-        <v>9.5299999999999994</v>
+        <v>9.61</v>
       </c>
       <c r="C49" s="11"/>
     </row>
@@ -34005,7 +35803,7 @@
         <v>17</v>
       </c>
       <c r="B50" s="5">
-        <v>17.68</v>
+        <v>18.64</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -34013,15 +35811,15 @@
         <v>20</v>
       </c>
       <c r="B51" s="7">
-        <v>4.0199999999999996</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>27</v>
+      <c r="B52" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -34029,7 +35827,7 @@
         <v>18</v>
       </c>
       <c r="B53" s="5">
-        <v>9.1</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -34037,7 +35835,7 @@
         <v>16</v>
       </c>
       <c r="B54" s="5">
-        <v>10.58</v>
+        <v>13.02</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -34045,7 +35843,7 @@
         <v>22</v>
       </c>
       <c r="B55" s="5">
-        <v>15.6</v>
+        <v>16.28</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -34053,7 +35851,7 @@
         <v>21</v>
       </c>
       <c r="B56" s="5">
-        <v>9.26</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -34061,7 +35859,7 @@
         <v>17</v>
       </c>
       <c r="B57" s="5">
-        <v>9.92</v>
+        <v>17.68</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -34069,6 +35867,62 @@
         <v>20</v>
       </c>
       <c r="B58" s="7">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="5">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="5">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="5">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="5">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="5">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="7">
         <v>2.65</v>
       </c>
     </row>

</xml_diff>